<commit_message>
Edits to RMD3 and Analysis_Progress
</commit_message>
<xml_diff>
--- a/Analysis_Progress.xlsx
+++ b/Analysis_Progress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9d4c4f1623d30376/Documents/GitHub/Rissos_Geographic_Variation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="592" documentId="8_{C4C2D1DD-6DD6-49C2-8C12-51DEE2FC981A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{830F13B4-C1D8-4CD9-B116-86BA90CAD00A}"/>
+  <xr:revisionPtr revIDLastSave="617" documentId="8_{C4C2D1DD-6DD6-49C2-8C12-51DEE2FC981A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44DB5C94-2BFD-4520-ABAA-650EA9243B62}"/>
   <bookViews>
-    <workbookView xWindow="2325" yWindow="0" windowWidth="10710" windowHeight="11895" xr2:uid="{8391C37B-1672-4229-8478-45F991E75901}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{8391C37B-1672-4229-8478-45F991E75901}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="56">
   <si>
     <t>PG_Click_Detections</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Add_Events_To_Database</t>
   </si>
   <si>
-    <t>Manual_Click_Verification</t>
-  </si>
-  <si>
     <t>Drift</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
     <t>ADRIFT_068</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Double check clicks look ok - initial PG was thick line of clicks</t>
   </si>
   <si>
@@ -113,9 +107,6 @@
     <t>Chunk 4 of RMD 2 took a LONG time</t>
   </si>
   <si>
-    <t>Add Files to Box</t>
-  </si>
-  <si>
     <t>RMD 1 taking a long time (multiple hours)</t>
   </si>
   <si>
@@ -198,6 +189,21 @@
   </si>
   <si>
     <t>Something wrong with this dirft</t>
+  </si>
+  <si>
+    <t>Spectrograms_And_Spectra</t>
+  </si>
+  <si>
+    <t>Add Acoustic Studies, Databases, and Binaries to Box</t>
+  </si>
+  <si>
+    <t>Add Spectrograms and Spectra to Box</t>
+  </si>
+  <si>
+    <t>General Notes</t>
+  </si>
+  <si>
+    <t>Notes on Spectrograms and Specta (Events worth looking into)</t>
   </si>
 </sst>
 </file>
@@ -349,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -402,10 +408,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -429,6 +431,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -768,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A18B98B-9FEB-4551-88CC-94F33BC1EF6E}">
-  <dimension ref="A1:BN129"/>
+  <dimension ref="A1:BP129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="41" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J82" sqref="J82"/>
+    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -780,56 +791,65 @@
     <col min="2" max="2" width="19.06640625" customWidth="1"/>
     <col min="3" max="3" width="29.19921875" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="10" width="24.1328125" customWidth="1"/>
-    <col min="11" max="11" width="50.73046875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.06640625" style="20"/>
+    <col min="5" max="9" width="24.1328125" customWidth="1"/>
+    <col min="10" max="10" width="44.265625" customWidth="1"/>
+    <col min="11" max="11" width="35.53125" customWidth="1"/>
+    <col min="12" max="12" width="53.86328125" customWidth="1"/>
+    <col min="13" max="13" width="50.73046875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.06640625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" s="13" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:68" s="34" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="E1" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" s="33"/>
+    </row>
+    <row r="2" spans="1:68" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="21"/>
-    </row>
-    <row r="2" spans="1:66" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2" s="2">
         <v>44403.170833333337</v>
@@ -838,19 +858,24 @@
         <v>44403.179166666669</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:66" s="4" customFormat="1" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+    </row>
+    <row r="3" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D3" s="5">
         <v>44407.519768518519</v>
       </c>
@@ -860,11 +885,12 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="20"/>
-      <c r="M3"/>
-      <c r="N3"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="20"/>
       <c r="O3"/>
       <c r="P3"/>
       <c r="Q3"/>
@@ -917,16 +943,18 @@
       <c r="BL3"/>
       <c r="BM3"/>
       <c r="BN3"/>
-    </row>
-    <row r="4" spans="1:66" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="BO3"/>
+      <c r="BP3"/>
+    </row>
+    <row r="4" spans="1:68" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" s="8">
         <v>44404.561458333337</v>
@@ -935,21 +963,22 @@
         <v>44404.602083333331</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" s="17"/>
-      <c r="L4" s="20"/>
-      <c r="M4"/>
-      <c r="N4"/>
+        <v>7</v>
+      </c>
+      <c r="I4" s="9"/>
+      <c r="J4" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="20"/>
       <c r="O4"/>
       <c r="P4"/>
       <c r="Q4"/>
@@ -1002,16 +1031,18 @@
       <c r="BL4"/>
       <c r="BM4"/>
       <c r="BN4"/>
-    </row>
-    <row r="5" spans="1:66" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="BO4"/>
+      <c r="BP4"/>
+    </row>
+    <row r="5" spans="1:68" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" s="8">
         <v>44360.256701388891</v>
@@ -1020,21 +1051,22 @@
         <v>44360.28528935185</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="K5" s="17"/>
-      <c r="L5" s="20"/>
-      <c r="M5"/>
-      <c r="N5"/>
+        <v>7</v>
+      </c>
+      <c r="I5" s="9"/>
+      <c r="J5" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="20"/>
       <c r="O5"/>
       <c r="P5"/>
       <c r="Q5"/>
@@ -1087,16 +1119,18 @@
       <c r="BL5"/>
       <c r="BM5"/>
       <c r="BN5"/>
-    </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="BO5"/>
+      <c r="BP5"/>
+    </row>
+    <row r="6" spans="1:68" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" s="2">
         <v>44580.109351851846</v>
@@ -1105,19 +1139,22 @@
         <v>44580.123611111107</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" s="28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+    </row>
+    <row r="7" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D7" s="2">
         <v>44580.177847222221</v>
       </c>
@@ -1127,9 +1164,12 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="J7" s="28"/>
-    </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="I7" s="3"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+    </row>
+    <row r="8" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D8" s="2">
         <v>44580.225891203707</v>
       </c>
@@ -1139,9 +1179,12 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="J8" s="28"/>
-    </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="I8" s="3"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+    </row>
+    <row r="9" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D9" s="2">
         <v>44580.253530092603</v>
       </c>
@@ -1151,9 +1194,12 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="J9" s="28"/>
-    </row>
-    <row r="10" spans="1:66" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="I9" s="3"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+    </row>
+    <row r="10" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D10" s="5">
         <v>44580.292696759258</v>
       </c>
@@ -1163,11 +1209,12 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="20"/>
-      <c r="M10"/>
-      <c r="N10"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="20"/>
       <c r="O10"/>
       <c r="P10"/>
       <c r="Q10"/>
@@ -1220,16 +1267,18 @@
       <c r="BL10"/>
       <c r="BM10"/>
       <c r="BN10"/>
-    </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="BO10"/>
+      <c r="BP10"/>
+    </row>
+    <row r="11" spans="1:68" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D11" s="2">
         <v>44735.246354166673</v>
@@ -1238,20 +1287,22 @@
         <v>44735.249305555553</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I11" s="3"/>
-      <c r="J11" s="28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:66" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="J11" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+    </row>
+    <row r="12" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D12" s="5">
         <v>44737.283750000002</v>
       </c>
@@ -1262,11 +1313,11 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="20"/>
-      <c r="M12"/>
-      <c r="N12"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="20"/>
       <c r="O12"/>
       <c r="P12"/>
       <c r="Q12"/>
@@ -1319,16 +1370,18 @@
       <c r="BL12"/>
       <c r="BM12"/>
       <c r="BN12"/>
-    </row>
-    <row r="13" spans="1:66" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="BO12"/>
+      <c r="BP12"/>
+    </row>
+    <row r="13" spans="1:68" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D13" s="8">
         <v>44818.156134259261</v>
@@ -1337,22 +1390,22 @@
         <v>44818.174768518518</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I13" s="9"/>
-      <c r="J13" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="K13" s="17"/>
-      <c r="L13" s="20"/>
-      <c r="M13"/>
-      <c r="N13"/>
+      <c r="J13" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="20"/>
       <c r="O13"/>
       <c r="P13"/>
       <c r="Q13"/>
@@ -1405,16 +1458,18 @@
       <c r="BL13"/>
       <c r="BM13"/>
       <c r="BN13"/>
-    </row>
-    <row r="14" spans="1:66" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="BO13"/>
+      <c r="BP13"/>
+    </row>
+    <row r="14" spans="1:68" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A14" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D14" s="8">
         <v>44818.185706018507</v>
@@ -1423,22 +1478,22 @@
         <v>44818.250856481478</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I14" s="9"/>
-      <c r="J14" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="K14" s="17"/>
-      <c r="L14" s="20"/>
-      <c r="M14"/>
-      <c r="N14"/>
+      <c r="J14" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="20"/>
       <c r="O14"/>
       <c r="P14"/>
       <c r="Q14"/>
@@ -1491,16 +1546,18 @@
       <c r="BL14"/>
       <c r="BM14"/>
       <c r="BN14"/>
-    </row>
-    <row r="15" spans="1:66" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="BO14"/>
+      <c r="BP14"/>
+    </row>
+    <row r="15" spans="1:68" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D15" s="8">
         <v>44882.326249999998</v>
@@ -1509,22 +1566,22 @@
         <v>44882.345405092587</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I15" s="9"/>
-      <c r="J15" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="K15" s="17"/>
-      <c r="L15" s="20"/>
-      <c r="M15"/>
-      <c r="N15"/>
+      <c r="J15" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="20"/>
       <c r="O15"/>
       <c r="P15"/>
       <c r="Q15"/>
@@ -1577,16 +1634,18 @@
       <c r="BL15"/>
       <c r="BM15"/>
       <c r="BN15"/>
-    </row>
-    <row r="16" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="BO15"/>
+      <c r="BP15"/>
+    </row>
+    <row r="16" spans="1:68" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D16" s="2">
         <v>44909.985347222217</v>
@@ -1595,20 +1654,22 @@
         <v>44910.02342592593</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I16" s="3"/>
-      <c r="J16" s="28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:66" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="J16" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+    </row>
+    <row r="17" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D17" s="5">
         <v>44910.070185185177</v>
       </c>
@@ -1619,11 +1680,11 @@
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="20"/>
-      <c r="M17"/>
-      <c r="N17"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="20"/>
       <c r="O17"/>
       <c r="P17"/>
       <c r="Q17"/>
@@ -1676,16 +1737,18 @@
       <c r="BL17"/>
       <c r="BM17"/>
       <c r="BN17"/>
-    </row>
-    <row r="18" spans="1:66" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="BO17"/>
+      <c r="BP17"/>
+    </row>
+    <row r="18" spans="1:68" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D18" s="8">
         <v>45005.351689814823</v>
@@ -1694,22 +1757,22 @@
         <v>45005.373553240737</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I18" s="9"/>
-      <c r="J18" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="K18" s="17"/>
-      <c r="L18" s="20"/>
-      <c r="M18"/>
-      <c r="N18"/>
+      <c r="J18" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="20"/>
       <c r="O18"/>
       <c r="P18"/>
       <c r="Q18"/>
@@ -1762,16 +1825,18 @@
       <c r="BL18"/>
       <c r="BM18"/>
       <c r="BN18"/>
-    </row>
-    <row r="19" spans="1:66" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="BO18"/>
+      <c r="BP18"/>
+    </row>
+    <row r="19" spans="1:68" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A19" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D19" s="8">
         <v>45005.294664351852</v>
@@ -1780,22 +1845,22 @@
         <v>45005.301898148136</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I19" s="9"/>
-      <c r="J19" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="K19" s="17"/>
-      <c r="L19" s="20"/>
-      <c r="M19"/>
-      <c r="N19"/>
+      <c r="J19" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="20"/>
       <c r="O19"/>
       <c r="P19"/>
       <c r="Q19"/>
@@ -1848,16 +1913,18 @@
       <c r="BL19"/>
       <c r="BM19"/>
       <c r="BN19"/>
-    </row>
-    <row r="20" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="BO19"/>
+      <c r="BP19"/>
+    </row>
+    <row r="20" spans="1:68" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D20" s="2">
         <v>45002.156157407408</v>
@@ -1866,23 +1933,25 @@
         <v>45002.260150462957</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I20" s="3"/>
-      <c r="J20" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="J20" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D21" s="2">
         <v>45002.272129629629</v>
       </c>
@@ -1893,12 +1962,14 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D22" s="2">
         <v>45002.29892361111</v>
       </c>
@@ -1909,9 +1980,11 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
-      <c r="J22" s="28"/>
-    </row>
-    <row r="23" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+    </row>
+    <row r="23" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D23" s="2">
         <v>45002.429236111107</v>
       </c>
@@ -1922,9 +1995,11 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
-      <c r="J23" s="28"/>
-    </row>
-    <row r="24" spans="1:66" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+    </row>
+    <row r="24" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D24" s="5">
         <v>45002.964166666672</v>
       </c>
@@ -1935,11 +2010,11 @@
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="20"/>
-      <c r="M24"/>
-      <c r="N24"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="20"/>
       <c r="O24"/>
       <c r="P24"/>
       <c r="Q24"/>
@@ -1992,16 +2067,18 @@
       <c r="BL24"/>
       <c r="BM24"/>
       <c r="BN24"/>
-    </row>
-    <row r="25" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="BO24"/>
+      <c r="BP24"/>
+    </row>
+    <row r="25" spans="1:68" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D25" s="2">
         <v>45002.077708333338</v>
@@ -2010,23 +2087,25 @@
         <v>45002.100451388891</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I25" s="3"/>
-      <c r="J25" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="J25" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D26" s="2">
         <v>45002.114224537043</v>
       </c>
@@ -2037,9 +2116,11 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
-      <c r="J26" s="28"/>
-    </row>
-    <row r="27" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+    </row>
+    <row r="27" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D27" s="2">
         <v>45002.160868055551</v>
       </c>
@@ -2050,9 +2131,11 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
-      <c r="J27" s="28"/>
-    </row>
-    <row r="28" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
+    </row>
+    <row r="28" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D28" s="2">
         <v>45002.342222222222</v>
       </c>
@@ -2063,9 +2146,11 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
-      <c r="J28" s="28"/>
-    </row>
-    <row r="29" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
+    </row>
+    <row r="29" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D29" s="2">
         <v>45002.523240740753</v>
       </c>
@@ -2076,9 +2161,11 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
-      <c r="J29" s="28"/>
-    </row>
-    <row r="30" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="J29" s="26"/>
+      <c r="K29" s="26"/>
+      <c r="L29" s="26"/>
+    </row>
+    <row r="30" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D30" s="2">
         <v>45003.08756944444</v>
       </c>
@@ -2089,9 +2176,11 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
-      <c r="J30" s="28"/>
-    </row>
-    <row r="31" spans="1:66" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="26"/>
+    </row>
+    <row r="31" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D31" s="5">
         <v>45003.336469907408</v>
       </c>
@@ -2102,11 +2191,11 @@
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
-      <c r="J31" s="29"/>
-      <c r="K31" s="16"/>
-      <c r="L31" s="20"/>
-      <c r="M31"/>
-      <c r="N31"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="27"/>
+      <c r="L31" s="27"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="20"/>
       <c r="O31"/>
       <c r="P31"/>
       <c r="Q31"/>
@@ -2159,16 +2248,18 @@
       <c r="BL31"/>
       <c r="BM31"/>
       <c r="BN31"/>
-    </row>
-    <row r="32" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="BO31"/>
+      <c r="BP31"/>
+    </row>
+    <row r="32" spans="1:68" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C32" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D32" s="2">
         <v>45002.345046296286</v>
@@ -2177,23 +2268,25 @@
         <v>45002.569745370369</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I32" s="3"/>
-      <c r="J32" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="J32" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D33" s="2">
         <v>45003.131979166668</v>
       </c>
@@ -2204,9 +2297,11 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
-      <c r="J33" s="28"/>
-    </row>
-    <row r="34" spans="1:66" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="J33" s="26"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="26"/>
+    </row>
+    <row r="34" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D34" s="5">
         <v>45003.354826388888</v>
       </c>
@@ -2217,11 +2312,11 @@
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
-      <c r="J34" s="29"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="20"/>
-      <c r="M34"/>
-      <c r="N34"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="27"/>
+      <c r="L34" s="27"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="20"/>
       <c r="O34"/>
       <c r="P34"/>
       <c r="Q34"/>
@@ -2274,16 +2369,18 @@
       <c r="BL34"/>
       <c r="BM34"/>
       <c r="BN34"/>
-    </row>
-    <row r="35" spans="1:66" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="BO34"/>
+      <c r="BP34"/>
+    </row>
+    <row r="35" spans="1:68" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A35" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D35" s="8">
         <v>45044.219282407408</v>
@@ -2292,22 +2389,22 @@
         <v>45044.23646990741</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H35" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="I35" s="9"/>
-      <c r="J35" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="K35" s="17"/>
-      <c r="L35" s="20"/>
-      <c r="M35"/>
-      <c r="N35"/>
+        <v>7</v>
+      </c>
+      <c r="H35" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="I35" s="25"/>
+      <c r="J35" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K35" s="28"/>
+      <c r="L35" s="28"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="20"/>
       <c r="O35"/>
       <c r="P35"/>
       <c r="Q35"/>
@@ -2360,16 +2457,18 @@
       <c r="BL35"/>
       <c r="BM35"/>
       <c r="BN35"/>
-    </row>
-    <row r="36" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="BO35"/>
+      <c r="BP35"/>
+    </row>
+    <row r="36" spans="1:68" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C36" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D36" s="2">
         <v>45054.301666666674</v>
@@ -2378,20 +2477,22 @@
         <v>45054.370532407411</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H36" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="I36" s="3"/>
-      <c r="J36" s="28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:66" s="4" customFormat="1" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="H36" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" s="25"/>
+      <c r="J36" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K36" s="26"/>
+      <c r="L36" s="26"/>
+    </row>
+    <row r="37" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D37" s="5">
         <v>45054.415324074071</v>
       </c>
@@ -2402,11 +2503,11 @@
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="16"/>
-      <c r="L37" s="20"/>
-      <c r="M37"/>
-      <c r="N37"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
+      <c r="L37" s="27"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="20"/>
       <c r="O37"/>
       <c r="P37"/>
       <c r="Q37"/>
@@ -2459,16 +2560,18 @@
       <c r="BL37"/>
       <c r="BM37"/>
       <c r="BN37"/>
-    </row>
-    <row r="38" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="BO37"/>
+      <c r="BP37"/>
+    </row>
+    <row r="38" spans="1:68" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B38" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C38" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D38" s="2">
         <v>45054.290162037039</v>
@@ -2477,20 +2580,22 @@
         <v>45054.302893518507</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I38" s="3"/>
-      <c r="J38" s="28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="J38" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K38" s="26"/>
+      <c r="L38" s="26"/>
+    </row>
+    <row r="39" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D39" s="2">
         <v>45054.415335648147</v>
       </c>
@@ -2501,9 +2606,11 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
-      <c r="J39" s="28"/>
-    </row>
-    <row r="40" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="J39" s="26"/>
+      <c r="K39" s="26"/>
+      <c r="L39" s="26"/>
+    </row>
+    <row r="40" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D40" s="2">
         <v>45055.170219907413</v>
       </c>
@@ -2514,9 +2621,11 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
-      <c r="J40" s="28"/>
-    </row>
-    <row r="41" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="J40" s="26"/>
+      <c r="K40" s="26"/>
+      <c r="L40" s="26"/>
+    </row>
+    <row r="41" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D41" s="2">
         <v>45055.351006944453</v>
       </c>
@@ -2527,9 +2636,11 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
-      <c r="J41" s="28"/>
-    </row>
-    <row r="42" spans="1:66" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="J41" s="26"/>
+      <c r="K41" s="26"/>
+      <c r="L41" s="26"/>
+    </row>
+    <row r="42" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D42" s="5">
         <v>45055.378020833326</v>
       </c>
@@ -2540,11 +2651,11 @@
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
-      <c r="J42" s="29"/>
-      <c r="K42" s="16"/>
-      <c r="L42" s="20"/>
-      <c r="M42"/>
-      <c r="N42"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="27"/>
+      <c r="L42" s="27"/>
+      <c r="M42" s="16"/>
+      <c r="N42" s="20"/>
       <c r="O42"/>
       <c r="P42"/>
       <c r="Q42"/>
@@ -2597,16 +2708,18 @@
       <c r="BL42"/>
       <c r="BM42"/>
       <c r="BN42"/>
-    </row>
-    <row r="43" spans="1:66" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="BO42"/>
+      <c r="BP42"/>
+    </row>
+    <row r="43" spans="1:68" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A43" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D43" s="8">
         <v>45128.184965277767</v>
@@ -2615,24 +2728,24 @@
         <v>45128.190115740741</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I43" s="9"/>
-      <c r="J43" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="K43" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="L43" s="20"/>
-      <c r="M43"/>
-      <c r="N43"/>
+      <c r="J43" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K43" s="28"/>
+      <c r="L43" s="28"/>
+      <c r="M43" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="N43" s="20"/>
       <c r="O43"/>
       <c r="P43"/>
       <c r="Q43"/>
@@ -2685,16 +2798,18 @@
       <c r="BL43"/>
       <c r="BM43"/>
       <c r="BN43"/>
-    </row>
-    <row r="44" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="BO43"/>
+      <c r="BP43"/>
+    </row>
+    <row r="44" spans="1:68" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B44" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C44" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D44" s="2">
         <v>45119.225254629629</v>
@@ -2703,20 +2818,22 @@
         <v>45119.260034722218</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I44" s="3"/>
-      <c r="J44" s="28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="J44" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K44" s="26"/>
+      <c r="L44" s="26"/>
+    </row>
+    <row r="45" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D45" s="2">
         <v>45119.310439814813</v>
       </c>
@@ -2727,9 +2844,11 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
-      <c r="J45" s="28"/>
-    </row>
-    <row r="46" spans="1:66" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="J45" s="26"/>
+      <c r="K45" s="26"/>
+      <c r="L45" s="26"/>
+    </row>
+    <row r="46" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D46" s="5">
         <v>45119.398460648154</v>
       </c>
@@ -2740,11 +2859,11 @@
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
-      <c r="J46" s="29"/>
-      <c r="K46" s="16"/>
-      <c r="L46" s="20"/>
-      <c r="M46"/>
-      <c r="N46"/>
+      <c r="J46" s="27"/>
+      <c r="K46" s="27"/>
+      <c r="L46" s="27"/>
+      <c r="M46" s="16"/>
+      <c r="N46" s="20"/>
       <c r="O46"/>
       <c r="P46"/>
       <c r="Q46"/>
@@ -2797,16 +2916,18 @@
       <c r="BL46"/>
       <c r="BM46"/>
       <c r="BN46"/>
-    </row>
-    <row r="47" spans="1:66" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="BO46"/>
+      <c r="BP46"/>
+    </row>
+    <row r="47" spans="1:68" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A47" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D47" s="8">
         <v>45122.301076388889</v>
@@ -2815,21 +2936,22 @@
         <v>45122.310162037043</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H47" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J47" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="K47" s="17"/>
-      <c r="L47" s="20"/>
-      <c r="M47"/>
-      <c r="N47"/>
+        <v>7</v>
+      </c>
+      <c r="I47" s="9"/>
+      <c r="J47" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K47" s="28"/>
+      <c r="L47" s="28"/>
+      <c r="M47" s="17"/>
+      <c r="N47" s="20"/>
       <c r="O47"/>
       <c r="P47"/>
       <c r="Q47"/>
@@ -2882,16 +3004,18 @@
       <c r="BL47"/>
       <c r="BM47"/>
       <c r="BN47"/>
-    </row>
-    <row r="48" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="BO47"/>
+      <c r="BP47"/>
+    </row>
+    <row r="48" spans="1:68" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B48" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C48" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D48" s="2">
         <v>45119.29614583333</v>
@@ -2900,19 +3024,22 @@
         <v>45119.330231481479</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J48" s="28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:66" s="4" customFormat="1" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="I48" s="3"/>
+      <c r="J48" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K48" s="26"/>
+      <c r="L48" s="26"/>
+    </row>
+    <row r="49" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D49" s="5">
         <v>45123.17931712963</v>
       </c>
@@ -2922,11 +3049,12 @@
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
-      <c r="J49" s="29"/>
-      <c r="K49" s="16"/>
-      <c r="L49" s="20"/>
-      <c r="M49"/>
-      <c r="N49"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="27"/>
+      <c r="K49" s="27"/>
+      <c r="L49" s="27"/>
+      <c r="M49" s="16"/>
+      <c r="N49" s="20"/>
       <c r="O49"/>
       <c r="P49"/>
       <c r="Q49"/>
@@ -2979,16 +3107,18 @@
       <c r="BL49"/>
       <c r="BM49"/>
       <c r="BN49"/>
-    </row>
-    <row r="50" spans="1:66" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="BO49"/>
+      <c r="BP49"/>
+    </row>
+    <row r="50" spans="1:68" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A50" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D50" s="8">
         <v>45143.215335648143</v>
@@ -2997,21 +3127,22 @@
         <v>45143.242708333331</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H50" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J50" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="K50" s="17"/>
-      <c r="L50" s="20"/>
-      <c r="M50"/>
-      <c r="N50"/>
+        <v>7</v>
+      </c>
+      <c r="I50" s="9"/>
+      <c r="J50" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K50" s="28"/>
+      <c r="L50" s="28"/>
+      <c r="M50" s="17"/>
+      <c r="N50" s="20"/>
       <c r="O50"/>
       <c r="P50"/>
       <c r="Q50"/>
@@ -3064,16 +3195,18 @@
       <c r="BL50"/>
       <c r="BM50"/>
       <c r="BN50"/>
-    </row>
-    <row r="51" spans="1:66" s="10" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="BO50"/>
+      <c r="BP50"/>
+    </row>
+    <row r="51" spans="1:68" s="10" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A51" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D51" s="11">
         <v>45166.222685185188</v>
@@ -3082,21 +3215,22 @@
         <v>45166.280787037038</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G51" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H51" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="J51" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="K51" s="18"/>
-      <c r="L51" s="20"/>
-      <c r="M51"/>
-      <c r="N51"/>
+        <v>7</v>
+      </c>
+      <c r="I51" s="12"/>
+      <c r="J51" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="K51" s="29"/>
+      <c r="L51" s="29"/>
+      <c r="M51" s="18"/>
+      <c r="N51" s="20"/>
       <c r="O51"/>
       <c r="P51"/>
       <c r="Q51"/>
@@ -3149,16 +3283,18 @@
       <c r="BL51"/>
       <c r="BM51"/>
       <c r="BN51"/>
-    </row>
-    <row r="52" spans="1:66" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="BO51"/>
+      <c r="BP51"/>
+    </row>
+    <row r="52" spans="1:68" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>42</v>
-      </c>
-      <c r="B52" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="C52" s="26" t="s">
-        <v>50</v>
+        <v>39</v>
+      </c>
+      <c r="B52" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52" s="24" t="s">
+        <v>47</v>
       </c>
       <c r="D52" s="2">
         <v>42612.580873842591</v>
@@ -3167,22 +3303,25 @@
         <v>42612.603443287036</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="J52" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="K52" s="33" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="53" spans="1:66" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+      <c r="I52" s="3"/>
+      <c r="J52" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="K52" s="26"/>
+      <c r="L52" s="26"/>
+      <c r="M52" s="31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D53" s="2">
         <v>42614.355943287039</v>
       </c>
@@ -3192,9 +3331,12 @@
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
-      <c r="J53" s="28"/>
-    </row>
-    <row r="54" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="I53" s="3"/>
+      <c r="J53" s="26"/>
+      <c r="K53" s="26"/>
+      <c r="L53" s="26"/>
+    </row>
+    <row r="54" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D54" s="2">
         <v>42615.103859953699</v>
       </c>
@@ -3204,9 +3346,12 @@
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
-      <c r="J54" s="28"/>
-    </row>
-    <row r="55" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="I54" s="3"/>
+      <c r="J54" s="26"/>
+      <c r="K54" s="26"/>
+      <c r="L54" s="26"/>
+    </row>
+    <row r="55" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D55" s="2">
         <v>42616.176603009248</v>
       </c>
@@ -3216,9 +3361,12 @@
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
-      <c r="J55" s="28"/>
-    </row>
-    <row r="56" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="I55" s="3"/>
+      <c r="J55" s="26"/>
+      <c r="K55" s="26"/>
+      <c r="L55" s="26"/>
+    </row>
+    <row r="56" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D56" s="2">
         <v>42616.414797453697</v>
       </c>
@@ -3228,9 +3376,12 @@
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
-      <c r="J56" s="28"/>
-    </row>
-    <row r="57" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="I56" s="3"/>
+      <c r="J56" s="26"/>
+      <c r="K56" s="26"/>
+      <c r="L56" s="26"/>
+    </row>
+    <row r="57" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D57" s="2">
         <v>42618.576927083333</v>
       </c>
@@ -3240,9 +3391,12 @@
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
-      <c r="J57" s="28"/>
-    </row>
-    <row r="58" spans="1:66" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="I57" s="3"/>
+      <c r="J57" s="26"/>
+      <c r="K57" s="26"/>
+      <c r="L57" s="26"/>
+    </row>
+    <row r="58" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D58" s="5">
         <v>42623.506336805563</v>
       </c>
@@ -3252,11 +3406,12 @@
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
       <c r="H58" s="6"/>
-      <c r="J58" s="29"/>
-      <c r="K58" s="16"/>
-      <c r="L58" s="20"/>
-      <c r="M58"/>
-      <c r="N58"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="27"/>
+      <c r="K58" s="27"/>
+      <c r="L58" s="27"/>
+      <c r="M58" s="16"/>
+      <c r="N58" s="20"/>
       <c r="O58"/>
       <c r="P58"/>
       <c r="Q58"/>
@@ -3309,16 +3464,18 @@
       <c r="BL58"/>
       <c r="BM58"/>
       <c r="BN58"/>
-    </row>
-    <row r="59" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="BO58"/>
+      <c r="BP58"/>
+    </row>
+    <row r="59" spans="1:68" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B59" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C59" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D59" s="2">
         <v>42612.561255787034</v>
@@ -3327,19 +3484,22 @@
         <v>42612.620804398153</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J59" s="28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:66" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="I59" s="3"/>
+      <c r="J59" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K59" s="26"/>
+      <c r="L59" s="26"/>
+    </row>
+    <row r="60" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D60" s="2">
         <v>42616.558420138877</v>
       </c>
@@ -3349,9 +3509,12 @@
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
-      <c r="J60" s="28"/>
-    </row>
-    <row r="61" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="I60" s="3"/>
+      <c r="J60" s="26"/>
+      <c r="K60" s="26"/>
+      <c r="L60" s="26"/>
+    </row>
+    <row r="61" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D61" s="2">
         <v>42617.194646990742</v>
       </c>
@@ -3361,9 +3524,12 @@
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
-      <c r="J61" s="28"/>
-    </row>
-    <row r="62" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="I61" s="3"/>
+      <c r="J61" s="26"/>
+      <c r="K61" s="26"/>
+      <c r="L61" s="26"/>
+    </row>
+    <row r="62" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D62" s="2">
         <v>42618.178038194441</v>
       </c>
@@ -3373,9 +3539,12 @@
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
-      <c r="J62" s="28"/>
-    </row>
-    <row r="63" spans="1:66" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="I62" s="3"/>
+      <c r="J62" s="26"/>
+      <c r="K62" s="26"/>
+      <c r="L62" s="26"/>
+    </row>
+    <row r="63" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D63" s="5">
         <v>42618.300086805553</v>
       </c>
@@ -3385,11 +3554,12 @@
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
       <c r="H63" s="6"/>
-      <c r="J63" s="29"/>
-      <c r="K63" s="16"/>
-      <c r="L63" s="20"/>
-      <c r="M63"/>
-      <c r="N63"/>
+      <c r="I63" s="6"/>
+      <c r="J63" s="27"/>
+      <c r="K63" s="27"/>
+      <c r="L63" s="27"/>
+      <c r="M63" s="16"/>
+      <c r="N63" s="20"/>
       <c r="O63"/>
       <c r="P63"/>
       <c r="Q63"/>
@@ -3442,16 +3612,18 @@
       <c r="BL63"/>
       <c r="BM63"/>
       <c r="BN63"/>
-    </row>
-    <row r="64" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="BO63"/>
+      <c r="BP63"/>
+    </row>
+    <row r="64" spans="1:68" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B64" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C64" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D64" s="2">
         <v>42612.348975694447</v>
@@ -3460,19 +3632,22 @@
         <v>42612.370908564822</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J64" s="28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="65" spans="1:66" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="I64" s="3"/>
+      <c r="J64" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K64" s="26"/>
+      <c r="L64" s="26"/>
+    </row>
+    <row r="65" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D65" s="2">
         <v>42612.474091435193</v>
       </c>
@@ -3482,9 +3657,12 @@
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
-      <c r="J65" s="28"/>
-    </row>
-    <row r="66" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="I65" s="3"/>
+      <c r="J65" s="26"/>
+      <c r="K65" s="26"/>
+      <c r="L65" s="26"/>
+    </row>
+    <row r="66" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D66" s="2">
         <v>42617.710376157411</v>
       </c>
@@ -3494,9 +3672,12 @@
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
-      <c r="J66" s="28"/>
-    </row>
-    <row r="67" spans="1:66" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="I66" s="3"/>
+      <c r="J66" s="26"/>
+      <c r="K66" s="26"/>
+      <c r="L66" s="26"/>
+    </row>
+    <row r="67" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D67" s="5">
         <v>42618.696718749998</v>
       </c>
@@ -3506,11 +3687,12 @@
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
       <c r="H67" s="6"/>
-      <c r="J67" s="29"/>
-      <c r="K67" s="16"/>
-      <c r="L67" s="20"/>
-      <c r="M67"/>
-      <c r="N67"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="27"/>
+      <c r="K67" s="27"/>
+      <c r="L67" s="27"/>
+      <c r="M67" s="16"/>
+      <c r="N67" s="20"/>
       <c r="O67"/>
       <c r="P67"/>
       <c r="Q67"/>
@@ -3563,16 +3745,18 @@
       <c r="BL67"/>
       <c r="BM67"/>
       <c r="BN67"/>
-    </row>
-    <row r="68" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="BO67"/>
+      <c r="BP67"/>
+    </row>
+    <row r="68" spans="1:68" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>44</v>
-      </c>
-      <c r="B68" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="C68" s="26" t="s">
-        <v>50</v>
+        <v>41</v>
+      </c>
+      <c r="B68" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C68" s="24" t="s">
+        <v>47</v>
       </c>
       <c r="D68" s="2">
         <v>42610.535399305547</v>
@@ -3581,22 +3765,25 @@
         <v>42610.555225694443</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="J68" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="K68" s="33" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="69" spans="1:66" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+      <c r="I68" s="3"/>
+      <c r="J68" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="K68" s="26"/>
+      <c r="L68" s="26"/>
+      <c r="M68" s="31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="69" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D69" s="2">
         <v>42612.31131365741</v>
       </c>
@@ -3606,9 +3793,12 @@
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
-      <c r="J69" s="28"/>
-    </row>
-    <row r="70" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="I69" s="3"/>
+      <c r="J69" s="26"/>
+      <c r="K69" s="26"/>
+      <c r="L69" s="26"/>
+    </row>
+    <row r="70" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D70" s="2">
         <v>42612.969021990742</v>
       </c>
@@ -3618,9 +3808,12 @@
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
-      <c r="J70" s="28"/>
-    </row>
-    <row r="71" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="I70" s="3"/>
+      <c r="J70" s="26"/>
+      <c r="K70" s="26"/>
+      <c r="L70" s="26"/>
+    </row>
+    <row r="71" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D71" s="2">
         <v>42616.257019675933</v>
       </c>
@@ -3630,9 +3823,12 @@
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
-      <c r="J71" s="28"/>
-    </row>
-    <row r="72" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="I71" s="3"/>
+      <c r="J71" s="26"/>
+      <c r="K71" s="26"/>
+      <c r="L71" s="26"/>
+    </row>
+    <row r="72" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D72" s="2">
         <v>42621.241869212958</v>
       </c>
@@ -3642,9 +3838,12 @@
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
-      <c r="J72" s="28"/>
-    </row>
-    <row r="73" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="I72" s="3"/>
+      <c r="J72" s="26"/>
+      <c r="K72" s="26"/>
+      <c r="L72" s="26"/>
+    </row>
+    <row r="73" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D73" s="2">
         <v>42623.419010416663</v>
       </c>
@@ -3654,9 +3853,12 @@
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
-      <c r="J73" s="28"/>
-    </row>
-    <row r="74" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="I73" s="3"/>
+      <c r="J73" s="26"/>
+      <c r="K73" s="26"/>
+      <c r="L73" s="26"/>
+    </row>
+    <row r="74" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D74" s="2">
         <v>42624.161082175917</v>
       </c>
@@ -3666,9 +3868,12 @@
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
-      <c r="J74" s="28"/>
-    </row>
-    <row r="75" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="I74" s="3"/>
+      <c r="J74" s="26"/>
+      <c r="K74" s="26"/>
+      <c r="L74" s="26"/>
+    </row>
+    <row r="75" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D75" s="2">
         <v>42626.26449652778</v>
       </c>
@@ -3678,9 +3883,12 @@
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
-      <c r="J75" s="28"/>
-    </row>
-    <row r="76" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="I75" s="3"/>
+      <c r="J75" s="26"/>
+      <c r="K75" s="26"/>
+      <c r="L75" s="26"/>
+    </row>
+    <row r="76" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D76" s="2">
         <v>42626.344184027781</v>
       </c>
@@ -3690,9 +3898,12 @@
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
-      <c r="J76" s="28"/>
-    </row>
-    <row r="77" spans="1:66" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="I76" s="3"/>
+      <c r="J76" s="26"/>
+      <c r="K76" s="26"/>
+      <c r="L76" s="26"/>
+    </row>
+    <row r="77" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D77" s="5">
         <v>42627.304484953696</v>
       </c>
@@ -3702,11 +3913,12 @@
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
       <c r="H77" s="6"/>
-      <c r="J77" s="29"/>
-      <c r="K77" s="16"/>
-      <c r="L77" s="20"/>
-      <c r="M77"/>
-      <c r="N77"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="27"/>
+      <c r="K77" s="27"/>
+      <c r="L77" s="27"/>
+      <c r="M77" s="16"/>
+      <c r="N77" s="20"/>
       <c r="O77"/>
       <c r="P77"/>
       <c r="Q77"/>
@@ -3759,16 +3971,18 @@
       <c r="BL77"/>
       <c r="BM77"/>
       <c r="BN77"/>
-    </row>
-    <row r="78" spans="1:66" x14ac:dyDescent="0.45">
+      <c r="BO77"/>
+      <c r="BP77"/>
+    </row>
+    <row r="78" spans="1:68" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B78" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C78" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D78" s="2">
         <v>42612.397146990741</v>
@@ -3777,19 +3991,22 @@
         <v>42612.39830439815</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J78" s="28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="79" spans="1:66" s="13" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+        <v>7</v>
+      </c>
+      <c r="I78" s="3"/>
+      <c r="J78" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K78" s="26"/>
+      <c r="L78" s="26"/>
+    </row>
+    <row r="79" spans="1:68" s="13" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D79" s="14">
         <v>42627.17509837963</v>
       </c>
@@ -3799,11 +4016,12 @@
       <c r="F79" s="15"/>
       <c r="G79" s="15"/>
       <c r="H79" s="15"/>
-      <c r="J79" s="32"/>
-      <c r="K79" s="19"/>
-      <c r="L79" s="20"/>
-      <c r="M79"/>
-      <c r="N79"/>
+      <c r="I79" s="15"/>
+      <c r="J79" s="30"/>
+      <c r="K79" s="30"/>
+      <c r="L79" s="30"/>
+      <c r="M79" s="19"/>
+      <c r="N79" s="20"/>
       <c r="O79"/>
       <c r="P79"/>
       <c r="Q79"/>
@@ -3856,525 +4074,668 @@
       <c r="BL79"/>
       <c r="BM79"/>
       <c r="BN79"/>
-    </row>
-    <row r="80" spans="1:66" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="BO79"/>
+      <c r="BP79"/>
+    </row>
+    <row r="80" spans="1:68" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B80" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C80" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D80" s="2">
         <v>43358.436255787034</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J80" s="28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="I80" s="3"/>
+      <c r="J80" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K80" s="26"/>
+      <c r="L80" s="26"/>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D81" s="2">
         <v>43358.450086805547</v>
       </c>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
-      <c r="J81" s="28"/>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I81" s="3"/>
+      <c r="J81" s="26"/>
+      <c r="K81" s="26"/>
+      <c r="L81" s="26"/>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D82" s="2">
         <v>43358.464033564807</v>
       </c>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
-      <c r="J82" s="28"/>
-    </row>
-    <row r="83" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="I82" s="3"/>
+      <c r="J82" s="26"/>
+      <c r="K82" s="26"/>
+      <c r="L82" s="26"/>
+    </row>
+    <row r="83" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D83" s="5">
         <v>43358.477864583328</v>
       </c>
       <c r="F83" s="6"/>
       <c r="G83" s="6"/>
       <c r="H83" s="6"/>
-      <c r="J83" s="29"/>
-      <c r="K83" s="16"/>
-      <c r="L83" s="24"/>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I83" s="6"/>
+      <c r="J83" s="27"/>
+      <c r="K83" s="27"/>
+      <c r="L83" s="27"/>
+      <c r="M83" s="16"/>
+      <c r="N83" s="22"/>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B84" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C84" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D84" s="2">
         <v>43338.193535879633</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J84" s="28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="I84" s="3"/>
+      <c r="J84" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K84" s="26"/>
+      <c r="L84" s="26"/>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D85" s="2">
         <v>43338.207309027777</v>
       </c>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
-      <c r="J85" s="28"/>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I85" s="3"/>
+      <c r="J85" s="26"/>
+      <c r="K85" s="26"/>
+      <c r="L85" s="26"/>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D86" s="2">
         <v>43339.263501157402</v>
       </c>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
-      <c r="J86" s="28"/>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I86" s="3"/>
+      <c r="J86" s="26"/>
+      <c r="K86" s="26"/>
+      <c r="L86" s="26"/>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D87" s="2">
         <v>43339.277042824076</v>
       </c>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
-      <c r="J87" s="28"/>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I87" s="3"/>
+      <c r="J87" s="26"/>
+      <c r="K87" s="26"/>
+      <c r="L87" s="26"/>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D88" s="2">
         <v>43339.290700231482</v>
       </c>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
-      <c r="J88" s="28"/>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I88" s="3"/>
+      <c r="J88" s="26"/>
+      <c r="K88" s="26"/>
+      <c r="L88" s="26"/>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D89" s="2">
         <v>43339.304589120373</v>
       </c>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
-      <c r="J89" s="28"/>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I89" s="3"/>
+      <c r="J89" s="26"/>
+      <c r="K89" s="26"/>
+      <c r="L89" s="26"/>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D90" s="2">
         <v>43339.734913194443</v>
       </c>
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
-      <c r="J90" s="28"/>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I90" s="3"/>
+      <c r="J90" s="26"/>
+      <c r="K90" s="26"/>
+      <c r="L90" s="26"/>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D91" s="2">
         <v>43339.749149305557</v>
       </c>
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
-      <c r="J91" s="28"/>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I91" s="3"/>
+      <c r="J91" s="26"/>
+      <c r="K91" s="26"/>
+      <c r="L91" s="26"/>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D92" s="2">
         <v>43344.179531250003</v>
       </c>
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
-      <c r="J92" s="28"/>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I92" s="3"/>
+      <c r="J92" s="26"/>
+      <c r="K92" s="26"/>
+      <c r="L92" s="26"/>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D93" s="2">
         <v>43344.193420138887</v>
       </c>
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
-      <c r="J93" s="28"/>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I93" s="3"/>
+      <c r="J93" s="26"/>
+      <c r="K93" s="26"/>
+      <c r="L93" s="26"/>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D94" s="2">
         <v>43345.248917824079</v>
       </c>
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
-      <c r="J94" s="28"/>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I94" s="3"/>
+      <c r="J94" s="26"/>
+      <c r="K94" s="26"/>
+      <c r="L94" s="26"/>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D95" s="2">
         <v>43345.262748842593</v>
       </c>
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
-      <c r="J95" s="28"/>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I95" s="3"/>
+      <c r="J95" s="26"/>
+      <c r="K95" s="26"/>
+      <c r="L95" s="26"/>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D96" s="2">
         <v>43345.2769849537</v>
       </c>
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
-      <c r="J96" s="28"/>
-    </row>
-    <row r="97" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="I96" s="3"/>
+      <c r="J96" s="26"/>
+      <c r="K96" s="26"/>
+      <c r="L96" s="26"/>
+    </row>
+    <row r="97" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D97" s="2">
         <v>43345.457366898147</v>
       </c>
       <c r="F97" s="3"/>
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
-      <c r="J97" s="28"/>
-    </row>
-    <row r="98" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="I97" s="3"/>
+      <c r="J97" s="26"/>
+      <c r="K97" s="26"/>
+      <c r="L97" s="26"/>
+    </row>
+    <row r="98" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D98" s="2">
         <v>43346.276753472222</v>
       </c>
       <c r="F98" s="3"/>
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
-      <c r="J98" s="28"/>
-    </row>
-    <row r="99" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="I98" s="3"/>
+      <c r="J98" s="26"/>
+      <c r="K98" s="26"/>
+      <c r="L98" s="26"/>
+    </row>
+    <row r="99" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D99" s="2">
         <v>43347.457482638893</v>
       </c>
       <c r="F99" s="3"/>
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
-      <c r="J99" s="28"/>
-    </row>
-    <row r="100" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="I99" s="3"/>
+      <c r="J99" s="26"/>
+      <c r="K99" s="26"/>
+      <c r="L99" s="26"/>
+    </row>
+    <row r="100" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D100" s="2">
         <v>43348.318304398148</v>
       </c>
       <c r="F100" s="3"/>
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
-      <c r="J100" s="28"/>
-    </row>
-    <row r="101" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="I100" s="3"/>
+      <c r="J100" s="26"/>
+      <c r="K100" s="26"/>
+      <c r="L100" s="26"/>
+    </row>
+    <row r="101" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D101" s="2">
         <v>43348.332193287039</v>
       </c>
       <c r="F101" s="3"/>
       <c r="G101" s="3"/>
       <c r="H101" s="3"/>
-      <c r="J101" s="28"/>
-    </row>
-    <row r="102" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="I101" s="3"/>
+      <c r="J101" s="26"/>
+      <c r="K101" s="26"/>
+      <c r="L101" s="26"/>
+    </row>
+    <row r="102" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D102" s="2">
         <v>43349.151695601853</v>
       </c>
       <c r="F102" s="3"/>
       <c r="G102" s="3"/>
       <c r="H102" s="3"/>
-      <c r="J102" s="28"/>
-    </row>
-    <row r="103" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="I102" s="3"/>
+      <c r="J102" s="26"/>
+      <c r="K102" s="26"/>
+      <c r="L102" s="26"/>
+    </row>
+    <row r="103" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D103" s="2">
         <v>43349.458234953709</v>
       </c>
       <c r="F103" s="3"/>
       <c r="G103" s="3"/>
       <c r="H103" s="3"/>
-      <c r="J103" s="28"/>
-    </row>
-    <row r="104" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="I103" s="3"/>
+      <c r="J103" s="26"/>
+      <c r="K103" s="26"/>
+      <c r="L103" s="26"/>
+    </row>
+    <row r="104" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D104" s="2">
         <v>43349.471487268507</v>
       </c>
       <c r="F104" s="3"/>
       <c r="G104" s="3"/>
       <c r="H104" s="3"/>
-      <c r="J104" s="28"/>
-    </row>
-    <row r="105" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="I104" s="3"/>
+      <c r="J104" s="26"/>
+      <c r="K104" s="26"/>
+      <c r="L104" s="26"/>
+    </row>
+    <row r="105" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D105" s="2">
         <v>43351.24909143518</v>
       </c>
       <c r="F105" s="3"/>
       <c r="G105" s="3"/>
       <c r="H105" s="3"/>
-      <c r="J105" s="28"/>
-    </row>
-    <row r="106" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="I105" s="3"/>
+      <c r="J105" s="26"/>
+      <c r="K105" s="26"/>
+      <c r="L105" s="26"/>
+    </row>
+    <row r="106" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D106" s="2">
         <v>43353.151637731477</v>
       </c>
       <c r="F106" s="3"/>
       <c r="G106" s="3"/>
       <c r="H106" s="3"/>
-      <c r="J106" s="28"/>
-    </row>
-    <row r="107" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="I106" s="3"/>
+      <c r="J106" s="26"/>
+      <c r="K106" s="26"/>
+      <c r="L106" s="26"/>
+    </row>
+    <row r="107" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D107" s="2">
         <v>43357.471313657406</v>
       </c>
       <c r="F107" s="3"/>
       <c r="G107" s="3"/>
       <c r="H107" s="3"/>
-      <c r="J107" s="28"/>
-    </row>
-    <row r="108" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="I107" s="3"/>
+      <c r="J107" s="26"/>
+      <c r="K107" s="26"/>
+      <c r="L107" s="26"/>
+    </row>
+    <row r="108" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D108" s="2">
         <v>43358.318188657402</v>
       </c>
       <c r="F108" s="3"/>
       <c r="G108" s="3"/>
       <c r="H108" s="3"/>
-      <c r="J108" s="28"/>
-    </row>
-    <row r="109" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="I108" s="3"/>
+      <c r="J108" s="26"/>
+      <c r="K108" s="26"/>
+      <c r="L108" s="26"/>
+    </row>
+    <row r="109" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D109" s="2">
         <v>43359.318651620371</v>
       </c>
       <c r="F109" s="3"/>
       <c r="G109" s="3"/>
       <c r="H109" s="3"/>
-      <c r="J109" s="28"/>
-    </row>
-    <row r="110" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="I109" s="3"/>
+      <c r="J109" s="26"/>
+      <c r="K109" s="26"/>
+      <c r="L109" s="26"/>
+    </row>
+    <row r="110" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D110" s="2">
         <v>43363.818651620371</v>
       </c>
       <c r="F110" s="3"/>
       <c r="G110" s="3"/>
       <c r="H110" s="3"/>
-      <c r="J110" s="28"/>
-    </row>
-    <row r="111" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="I110" s="3"/>
+      <c r="J110" s="26"/>
+      <c r="K110" s="26"/>
+      <c r="L110" s="26"/>
+    </row>
+    <row r="111" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D111" s="2">
         <v>43367.123802083333</v>
       </c>
       <c r="F111" s="3"/>
       <c r="G111" s="3"/>
       <c r="H111" s="3"/>
-      <c r="J111" s="28"/>
-    </row>
-    <row r="112" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="I111" s="3"/>
+      <c r="J111" s="26"/>
+      <c r="K111" s="26"/>
+      <c r="L111" s="26"/>
+    </row>
+    <row r="112" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D112" s="2">
         <v>43367.138211805563</v>
       </c>
       <c r="F112" s="3"/>
       <c r="G112" s="3"/>
       <c r="H112" s="3"/>
-      <c r="J112" s="28"/>
-    </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I112" s="3"/>
+      <c r="J112" s="26"/>
+      <c r="K112" s="26"/>
+      <c r="L112" s="26"/>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D113" s="2">
         <v>43367.151695601853</v>
       </c>
       <c r="F113" s="3"/>
       <c r="G113" s="3"/>
       <c r="H113" s="3"/>
-      <c r="J113" s="28"/>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I113" s="3"/>
+      <c r="J113" s="26"/>
+      <c r="K113" s="26"/>
+      <c r="L113" s="26"/>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D114" s="2">
         <v>43368.346197916668</v>
       </c>
       <c r="F114" s="3"/>
       <c r="G114" s="3"/>
       <c r="H114" s="3"/>
-      <c r="J114" s="28"/>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I114" s="3"/>
+      <c r="J114" s="26"/>
+      <c r="K114" s="26"/>
+      <c r="L114" s="26"/>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D115" s="2">
         <v>43368.359971064812</v>
       </c>
       <c r="F115" s="3"/>
       <c r="G115" s="3"/>
       <c r="H115" s="3"/>
-      <c r="J115" s="28"/>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I115" s="3"/>
+      <c r="J115" s="26"/>
+      <c r="K115" s="26"/>
+      <c r="L115" s="26"/>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D116" s="2">
         <v>43370.290642361113</v>
       </c>
       <c r="F116" s="3"/>
       <c r="G116" s="3"/>
       <c r="H116" s="3"/>
-      <c r="J116" s="28"/>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I116" s="3"/>
+      <c r="J116" s="26"/>
+      <c r="K116" s="26"/>
+      <c r="L116" s="26"/>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D117" s="2">
         <v>43370.304704861112</v>
       </c>
       <c r="F117" s="3"/>
       <c r="G117" s="3"/>
       <c r="H117" s="3"/>
-      <c r="J117" s="28"/>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I117" s="3"/>
+      <c r="J117" s="26"/>
+      <c r="K117" s="26"/>
+      <c r="L117" s="26"/>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D118" s="2">
         <v>43370.373859953703</v>
       </c>
       <c r="F118" s="3"/>
       <c r="G118" s="3"/>
       <c r="H118" s="3"/>
-      <c r="J118" s="28"/>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I118" s="3"/>
+      <c r="J118" s="26"/>
+      <c r="K118" s="26"/>
+      <c r="L118" s="26"/>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D119" s="2">
         <v>43370.401753472222</v>
       </c>
       <c r="F119" s="3"/>
       <c r="G119" s="3"/>
       <c r="H119" s="3"/>
-      <c r="J119" s="28"/>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I119" s="3"/>
+      <c r="J119" s="26"/>
+      <c r="K119" s="26"/>
+      <c r="L119" s="26"/>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D120" s="2">
         <v>43370.41587384259</v>
       </c>
       <c r="F120" s="3"/>
       <c r="G120" s="3"/>
       <c r="H120" s="3"/>
-      <c r="J120" s="28"/>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I120" s="3"/>
+      <c r="J120" s="26"/>
+      <c r="K120" s="26"/>
+      <c r="L120" s="26"/>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D121" s="2">
         <v>43372.929473379627</v>
       </c>
       <c r="F121" s="3"/>
       <c r="G121" s="3"/>
       <c r="H121" s="3"/>
-      <c r="J121" s="28"/>
-    </row>
-    <row r="122" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="I121" s="3"/>
+      <c r="J121" s="26"/>
+      <c r="K121" s="26"/>
+      <c r="L121" s="26"/>
+    </row>
+    <row r="122" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D122" s="5">
         <v>43372.943709490741</v>
       </c>
       <c r="F122" s="6"/>
       <c r="G122" s="6"/>
       <c r="H122" s="6"/>
-      <c r="J122" s="29"/>
-      <c r="K122" s="16"/>
-      <c r="L122" s="24"/>
-    </row>
-    <row r="123" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="I122" s="6"/>
+      <c r="J122" s="27"/>
+      <c r="K122" s="27"/>
+      <c r="L122" s="27"/>
+      <c r="M122" s="16"/>
+      <c r="N122" s="22"/>
+    </row>
+    <row r="123" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A123" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C123" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D123" s="8">
         <v>43353.138153935193</v>
       </c>
-      <c r="F123" s="27" t="s">
-        <v>8</v>
+      <c r="F123" s="25" t="s">
+        <v>7</v>
       </c>
       <c r="G123" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H123" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I123" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J123" s="30"/>
-      <c r="K123" s="17"/>
-      <c r="L123" s="25"/>
-    </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="I123" s="9"/>
+      <c r="J123" s="28"/>
+      <c r="K123" s="28"/>
+      <c r="L123" s="28"/>
+      <c r="M123" s="17"/>
+      <c r="N123" s="23"/>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B124" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C124" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D124" s="2">
         <v>43369.178304398149</v>
       </c>
-      <c r="F124" s="27" t="s">
-        <v>8</v>
+      <c r="F124" s="25" t="s">
+        <v>7</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H124" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I124" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J124" s="28"/>
-    </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="I124" s="3"/>
+      <c r="J124" s="26"/>
+      <c r="K124" s="26"/>
+      <c r="L124" s="26"/>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D125" s="2">
         <v>43369.192193287032</v>
       </c>
       <c r="F125" s="3"/>
       <c r="G125" s="3"/>
       <c r="H125" s="3"/>
-      <c r="J125" s="28"/>
-    </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I125" s="3"/>
+      <c r="J125" s="26"/>
+      <c r="K125" s="26"/>
+      <c r="L125" s="26"/>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D126" s="2">
         <v>43369.219971064813</v>
       </c>
       <c r="F126" s="3"/>
       <c r="G126" s="3"/>
       <c r="H126" s="3"/>
-      <c r="J126" s="28"/>
-    </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="I126" s="3"/>
+      <c r="J126" s="26"/>
+      <c r="K126" s="26"/>
+      <c r="L126" s="26"/>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D127" s="2">
         <v>43369.733802083327</v>
       </c>
       <c r="F127" s="3"/>
       <c r="G127" s="3"/>
       <c r="H127" s="3"/>
-      <c r="J127" s="28"/>
-    </row>
-    <row r="128" spans="1:12" s="13" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="I127" s="3"/>
+      <c r="J127" s="26"/>
+      <c r="K127" s="26"/>
+      <c r="L127" s="26"/>
+    </row>
+    <row r="128" spans="1:14" s="13" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D128" s="14">
         <v>43370.192251157408</v>
       </c>
       <c r="F128" s="15"/>
       <c r="G128" s="15"/>
       <c r="H128" s="15"/>
-      <c r="J128" s="32"/>
-      <c r="K128" s="19"/>
-      <c r="L128" s="21"/>
+      <c r="I128" s="15"/>
+      <c r="J128" s="30"/>
+      <c r="K128" s="30"/>
+      <c r="L128" s="30"/>
+      <c r="M128" s="19"/>
+      <c r="N128" s="21"/>
     </row>
     <row r="129" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>

</xml_diff>

<commit_message>
Updates to Analysis Progress
Completed the creation of Spectra and Spectrograms
</commit_message>
<xml_diff>
--- a/Analysis_Progress.xlsx
+++ b/Analysis_Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9d4c4f1623d30376/Documents/GitHub/Rissos_Geographic_Variation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="617" documentId="8_{C4C2D1DD-6DD6-49C2-8C12-51DEE2FC981A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44DB5C94-2BFD-4520-ABAA-650EA9243B62}"/>
+  <xr:revisionPtr revIDLastSave="742" documentId="8_{C4C2D1DD-6DD6-49C2-8C12-51DEE2FC981A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{679E015A-7CB2-4D96-A4EA-A320EE602669}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{8391C37B-1672-4229-8478-45F991E75901}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="72">
   <si>
     <t>PG_Click_Detections</t>
   </si>
@@ -204,6 +204,88 @@
   </si>
   <si>
     <t>Notes on Spectrograms and Specta (Events worth looking into)</t>
+  </si>
+  <si>
+    <t>Look into Event_001 further</t>
+  </si>
+  <si>
+    <t>Low number of clicks in Event_001</t>
+  </si>
+  <si>
+    <t>Look into Event_001 further - big chunks of dark</t>
+  </si>
+  <si>
+    <t>Look into Event_001 further - first third of Event_001 messy</t>
+  </si>
+  <si>
+    <t>Look into Event_001 and event_002 further - messy banding / missing banding</t>
+  </si>
+  <si>
+    <t>Look into Event_001 - messy</t>
+  </si>
+  <si>
+    <t>Look into Event_001 and Event_004 further</t>
+  </si>
+  <si>
+    <t>Look into Event_001 and Event_002 further</t>
+  </si>
+  <si>
+    <t>Look into Event_003, Event_004 (no spectral banding at all) and  Event_005 further</t>
+  </si>
+  <si>
+    <t>Look into Event_001 and Event_002 further - low number of clicks in Event_002</t>
+  </si>
+  <si>
+    <t>All Events need review - something really weird is going on here</t>
+  </si>
+  <si>
+    <t>All Events need review</t>
+  </si>
+  <si>
+    <t>Look into Event_001 (messy) and Event_002 (no banding) further</t>
+  </si>
+  <si>
+    <t>Look into Event_001 (messy), Event_002 (low click count), Event_003, Event_004 (low click count), and Event_005 further</t>
+  </si>
+  <si>
+    <t>Low number of clicks in Event_003</t>
+  </si>
+  <si>
+    <t>Look into following Events further (almost all of them): 
+Event_001 - low click count
+Event_002 - patchy banding
+Event_003 - low click count
+Event_004 - patchy banding
+Event_005 - patchy banding
+Event_006 - patchy banding
+Event_007 - low click count
+Event_008 - low click count
+Event_009 - patchy banding
+Event_011 - patchy banding
+Event_012 - patchy banding
+Event_013 - low click count
+Event_014 - low click count
+Event_015 - patchy banding
+Event_016 - low click count
+Event_017 - low click count
+Event_018 -low click count
+Event_019 - low click count
+Event_020 - low click count
+Event_021 - low click count
+Event_022 - patchy banding
+Event_023 - low click count
+Event_027 - low click count
+Event_028 - low click count
+Event_030 - low click count
+Event_031 - patchy banding
+Event_032 - patchy banding
+Event_033 - patchy banding
+Event_034 - patchy banding
+Event_035 - low click count
+Event_036 - patchy banding
+Event_037 - low click count
+Event_038 - low click count
+Event_039 - low click count</t>
   </si>
 </sst>
 </file>
@@ -213,7 +295,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss\ \U\T\C"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,6 +313,21 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -355,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -410,7 +507,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -429,9 +525,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -440,6 +533,91 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -781,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A18B98B-9FEB-4551-88CC-94F33BC1EF6E}">
   <dimension ref="A1:BP129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="D101" zoomScale="54" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -794,52 +972,52 @@
     <col min="5" max="9" width="24.1328125" customWidth="1"/>
     <col min="10" max="10" width="44.265625" customWidth="1"/>
     <col min="11" max="11" width="35.53125" customWidth="1"/>
-    <col min="12" max="12" width="53.86328125" customWidth="1"/>
+    <col min="12" max="12" width="97.73046875" style="1" customWidth="1"/>
     <col min="13" max="13" width="50.73046875" style="1" customWidth="1"/>
     <col min="14" max="14" width="9.06640625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" s="34" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:68" s="32" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="I1" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="K1" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="L1" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="M1" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="33"/>
+      <c r="N1" s="31"/>
     </row>
     <row r="2" spans="1:68" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
@@ -869,11 +1047,11 @@
       <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
+      <c r="J2" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="25"/>
+      <c r="L2" s="46"/>
     </row>
     <row r="3" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D3" s="5">
@@ -886,9 +1064,9 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="48"/>
       <c r="M3" s="16"/>
       <c r="N3" s="20"/>
       <c r="O3"/>
@@ -971,12 +1149,16 @@
       <c r="H4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
+      <c r="I4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="27"/>
+      <c r="L4" s="45" t="s">
+        <v>58</v>
+      </c>
       <c r="M4" s="17"/>
       <c r="N4" s="20"/>
       <c r="O4"/>
@@ -1059,12 +1241,14 @@
       <c r="H5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
+      <c r="I5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="27"/>
+      <c r="L5" s="45"/>
       <c r="M5" s="17"/>
       <c r="N5" s="20"/>
       <c r="O5"/>
@@ -1122,153 +1306,165 @@
       <c r="BO5"/>
       <c r="BP5"/>
     </row>
-    <row r="6" spans="1:68" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+    <row r="6" spans="1:68" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="34">
         <v>44580.109351851846</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="34">
         <v>44580.123611111107</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-    </row>
-    <row r="7" spans="1:68" x14ac:dyDescent="0.45">
-      <c r="D7" s="2">
+      <c r="F6" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="36"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="N6" s="38"/>
+    </row>
+    <row r="7" spans="1:68" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D7" s="34">
         <v>44580.177847222221</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="34">
         <v>44580.200335648136</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-    </row>
-    <row r="8" spans="1:68" x14ac:dyDescent="0.45">
-      <c r="D8" s="2">
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="38"/>
+    </row>
+    <row r="8" spans="1:68" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D8" s="34">
         <v>44580.225891203707</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="34">
         <v>44580.245625000003</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-    </row>
-    <row r="9" spans="1:68" x14ac:dyDescent="0.45">
-      <c r="D9" s="2">
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="38"/>
+    </row>
+    <row r="9" spans="1:68" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D9" s="34">
         <v>44580.253530092603</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="34">
         <v>44580.272847222222</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-    </row>
-    <row r="10" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="D10" s="5">
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="38"/>
+    </row>
+    <row r="10" spans="1:68" s="39" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D10" s="40">
         <v>44580.292696759258</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="40">
         <v>44580.323900462958</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="20"/>
-      <c r="O10"/>
-      <c r="P10"/>
-      <c r="Q10"/>
-      <c r="R10"/>
-      <c r="S10"/>
-      <c r="T10"/>
-      <c r="U10"/>
-      <c r="V10"/>
-      <c r="W10"/>
-      <c r="X10"/>
-      <c r="Y10"/>
-      <c r="Z10"/>
-      <c r="AA10"/>
-      <c r="AB10"/>
-      <c r="AC10"/>
-      <c r="AD10"/>
-      <c r="AE10"/>
-      <c r="AF10"/>
-      <c r="AG10"/>
-      <c r="AH10"/>
-      <c r="AI10"/>
-      <c r="AJ10"/>
-      <c r="AK10"/>
-      <c r="AL10"/>
-      <c r="AM10"/>
-      <c r="AN10"/>
-      <c r="AO10"/>
-      <c r="AP10"/>
-      <c r="AQ10"/>
-      <c r="AR10"/>
-      <c r="AS10"/>
-      <c r="AT10"/>
-      <c r="AU10"/>
-      <c r="AV10"/>
-      <c r="AW10"/>
-      <c r="AX10"/>
-      <c r="AY10"/>
-      <c r="AZ10"/>
-      <c r="BA10"/>
-      <c r="BB10"/>
-      <c r="BC10"/>
-      <c r="BD10"/>
-      <c r="BE10"/>
-      <c r="BF10"/>
-      <c r="BG10"/>
-      <c r="BH10"/>
-      <c r="BI10"/>
-      <c r="BJ10"/>
-      <c r="BK10"/>
-      <c r="BL10"/>
-      <c r="BM10"/>
-      <c r="BN10"/>
-      <c r="BO10"/>
-      <c r="BP10"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="33"/>
+      <c r="R10" s="33"/>
+      <c r="S10" s="33"/>
+      <c r="T10" s="33"/>
+      <c r="U10" s="33"/>
+      <c r="V10" s="33"/>
+      <c r="W10" s="33"/>
+      <c r="X10" s="33"/>
+      <c r="Y10" s="33"/>
+      <c r="Z10" s="33"/>
+      <c r="AA10" s="33"/>
+      <c r="AB10" s="33"/>
+      <c r="AC10" s="33"/>
+      <c r="AD10" s="33"/>
+      <c r="AE10" s="33"/>
+      <c r="AF10" s="33"/>
+      <c r="AG10" s="33"/>
+      <c r="AH10" s="33"/>
+      <c r="AI10" s="33"/>
+      <c r="AJ10" s="33"/>
+      <c r="AK10" s="33"/>
+      <c r="AL10" s="33"/>
+      <c r="AM10" s="33"/>
+      <c r="AN10" s="33"/>
+      <c r="AO10" s="33"/>
+      <c r="AP10" s="33"/>
+      <c r="AQ10" s="33"/>
+      <c r="AR10" s="33"/>
+      <c r="AS10" s="33"/>
+      <c r="AT10" s="33"/>
+      <c r="AU10" s="33"/>
+      <c r="AV10" s="33"/>
+      <c r="AW10" s="33"/>
+      <c r="AX10" s="33"/>
+      <c r="AY10" s="33"/>
+      <c r="AZ10" s="33"/>
+      <c r="BA10" s="33"/>
+      <c r="BB10" s="33"/>
+      <c r="BC10" s="33"/>
+      <c r="BD10" s="33"/>
+      <c r="BE10" s="33"/>
+      <c r="BF10" s="33"/>
+      <c r="BG10" s="33"/>
+      <c r="BH10" s="33"/>
+      <c r="BI10" s="33"/>
+      <c r="BJ10" s="33"/>
+      <c r="BK10" s="33"/>
+      <c r="BL10" s="33"/>
+      <c r="BM10" s="33"/>
+      <c r="BN10" s="33"/>
+      <c r="BO10" s="33"/>
+      <c r="BP10" s="33"/>
     </row>
     <row r="11" spans="1:68" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
@@ -1295,12 +1491,16 @@
       <c r="H11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
+      <c r="I11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" s="25"/>
+      <c r="L11" s="46" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="12" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D12" s="5">
@@ -1313,9 +1513,9 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="48"/>
       <c r="M12" s="16"/>
       <c r="N12" s="20"/>
       <c r="O12"/>
@@ -1398,12 +1598,14 @@
       <c r="H13" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="9"/>
-      <c r="J13" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
+      <c r="I13" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" s="27"/>
+      <c r="L13" s="45"/>
       <c r="M13" s="17"/>
       <c r="N13" s="20"/>
       <c r="O13"/>
@@ -1486,12 +1688,14 @@
       <c r="H14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="9"/>
-      <c r="J14" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
+      <c r="I14" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="K14" s="27"/>
+      <c r="L14" s="45"/>
       <c r="M14" s="17"/>
       <c r="N14" s="20"/>
       <c r="O14"/>
@@ -1574,12 +1778,16 @@
       <c r="H15" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
+      <c r="I15" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="K15" s="27"/>
+      <c r="L15" s="45" t="s">
+        <v>59</v>
+      </c>
       <c r="M15" s="17"/>
       <c r="N15" s="20"/>
       <c r="O15"/>
@@ -1662,12 +1870,16 @@
       <c r="H16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
+      <c r="I16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" s="25"/>
+      <c r="L16" s="46" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="17" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D17" s="5">
@@ -1680,9 +1892,9 @@
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="48"/>
       <c r="M17" s="16"/>
       <c r="N17" s="20"/>
       <c r="O17"/>
@@ -1740,93 +1952,95 @@
       <c r="BO17"/>
       <c r="BP17"/>
     </row>
-    <row r="18" spans="1:68" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="7" t="s">
+    <row r="18" spans="1:68" s="58" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="59">
         <v>45005.351689814823</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="59">
         <v>45005.373553240737</v>
       </c>
-      <c r="F18" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I18" s="9"/>
-      <c r="J18" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="20"/>
-      <c r="O18"/>
-      <c r="P18"/>
-      <c r="Q18"/>
-      <c r="R18"/>
-      <c r="S18"/>
-      <c r="T18"/>
-      <c r="U18"/>
-      <c r="V18"/>
-      <c r="W18"/>
-      <c r="X18"/>
-      <c r="Y18"/>
-      <c r="Z18"/>
-      <c r="AA18"/>
-      <c r="AB18"/>
-      <c r="AC18"/>
-      <c r="AD18"/>
-      <c r="AE18"/>
-      <c r="AF18"/>
-      <c r="AG18"/>
-      <c r="AH18"/>
-      <c r="AI18"/>
-      <c r="AJ18"/>
-      <c r="AK18"/>
-      <c r="AL18"/>
-      <c r="AM18"/>
-      <c r="AN18"/>
-      <c r="AO18"/>
-      <c r="AP18"/>
-      <c r="AQ18"/>
-      <c r="AR18"/>
-      <c r="AS18"/>
-      <c r="AT18"/>
-      <c r="AU18"/>
-      <c r="AV18"/>
-      <c r="AW18"/>
-      <c r="AX18"/>
-      <c r="AY18"/>
-      <c r="AZ18"/>
-      <c r="BA18"/>
-      <c r="BB18"/>
-      <c r="BC18"/>
-      <c r="BD18"/>
-      <c r="BE18"/>
-      <c r="BF18"/>
-      <c r="BG18"/>
-      <c r="BH18"/>
-      <c r="BI18"/>
-      <c r="BJ18"/>
-      <c r="BK18"/>
-      <c r="BL18"/>
-      <c r="BM18"/>
-      <c r="BN18"/>
-      <c r="BO18"/>
-      <c r="BP18"/>
+      <c r="F18" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="K18" s="27"/>
+      <c r="L18" s="53"/>
+      <c r="M18" s="45"/>
+      <c r="N18" s="60"/>
+      <c r="O18" s="61"/>
+      <c r="P18" s="61"/>
+      <c r="Q18" s="61"/>
+      <c r="R18" s="61"/>
+      <c r="S18" s="61"/>
+      <c r="T18" s="61"/>
+      <c r="U18" s="61"/>
+      <c r="V18" s="61"/>
+      <c r="W18" s="61"/>
+      <c r="X18" s="61"/>
+      <c r="Y18" s="61"/>
+      <c r="Z18" s="61"/>
+      <c r="AA18" s="61"/>
+      <c r="AB18" s="61"/>
+      <c r="AC18" s="61"/>
+      <c r="AD18" s="61"/>
+      <c r="AE18" s="61"/>
+      <c r="AF18" s="61"/>
+      <c r="AG18" s="61"/>
+      <c r="AH18" s="61"/>
+      <c r="AI18" s="61"/>
+      <c r="AJ18" s="61"/>
+      <c r="AK18" s="61"/>
+      <c r="AL18" s="61"/>
+      <c r="AM18" s="61"/>
+      <c r="AN18" s="61"/>
+      <c r="AO18" s="61"/>
+      <c r="AP18" s="61"/>
+      <c r="AQ18" s="61"/>
+      <c r="AR18" s="61"/>
+      <c r="AS18" s="61"/>
+      <c r="AT18" s="61"/>
+      <c r="AU18" s="61"/>
+      <c r="AV18" s="61"/>
+      <c r="AW18" s="61"/>
+      <c r="AX18" s="61"/>
+      <c r="AY18" s="61"/>
+      <c r="AZ18" s="61"/>
+      <c r="BA18" s="61"/>
+      <c r="BB18" s="61"/>
+      <c r="BC18" s="61"/>
+      <c r="BD18" s="61"/>
+      <c r="BE18" s="61"/>
+      <c r="BF18" s="61"/>
+      <c r="BG18" s="61"/>
+      <c r="BH18" s="61"/>
+      <c r="BI18" s="61"/>
+      <c r="BJ18" s="61"/>
+      <c r="BK18" s="61"/>
+      <c r="BL18" s="61"/>
+      <c r="BM18" s="61"/>
+      <c r="BN18" s="61"/>
+      <c r="BO18" s="61"/>
+      <c r="BP18" s="61"/>
     </row>
     <row r="19" spans="1:68" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A19" s="7" t="s">
@@ -1853,12 +2067,14 @@
       <c r="H19" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I19" s="9"/>
-      <c r="J19" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
+      <c r="I19" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="K19" s="27"/>
+      <c r="L19" s="45"/>
       <c r="M19" s="17"/>
       <c r="N19" s="20"/>
       <c r="O19"/>
@@ -1941,12 +2157,16 @@
       <c r="H20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
+      <c r="I20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="K20" s="25"/>
+      <c r="L20" s="46" t="s">
+        <v>69</v>
+      </c>
       <c r="M20" s="1" t="s">
         <v>16</v>
       </c>
@@ -1962,9 +2182,9 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="46"/>
       <c r="M21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1980,9 +2200,9 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="46"/>
     </row>
     <row r="23" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D23" s="2">
@@ -1995,9 +2215,9 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="46"/>
     </row>
     <row r="24" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D24" s="5">
@@ -2010,9 +2230,9 @@
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="48"/>
       <c r="M24" s="16"/>
       <c r="N24" s="20"/>
       <c r="O24"/>
@@ -2095,12 +2315,16 @@
       <c r="H25" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I25" s="3"/>
-      <c r="J25" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
+      <c r="I25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J25" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="K25" s="25"/>
+      <c r="L25" s="46" t="s">
+        <v>68</v>
+      </c>
       <c r="M25" s="1" t="s">
         <v>23</v>
       </c>
@@ -2116,9 +2340,9 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="26"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="46"/>
     </row>
     <row r="27" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D27" s="2">
@@ -2131,9 +2355,9 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="26"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="25"/>
+      <c r="L27" s="46"/>
     </row>
     <row r="28" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D28" s="2">
@@ -2146,9 +2370,9 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="25"/>
+      <c r="L28" s="46"/>
     </row>
     <row r="29" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D29" s="2">
@@ -2161,9 +2385,9 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="26"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="25"/>
+      <c r="L29" s="46"/>
     </row>
     <row r="30" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D30" s="2">
@@ -2176,9 +2400,9 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="26"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="25"/>
+      <c r="L30" s="46"/>
     </row>
     <row r="31" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D31" s="5">
@@ -2191,9 +2415,9 @@
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="27"/>
-      <c r="L31" s="27"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="48"/>
       <c r="M31" s="16"/>
       <c r="N31" s="20"/>
       <c r="O31"/>
@@ -2251,40 +2475,45 @@
       <c r="BO31"/>
       <c r="BP31"/>
     </row>
-    <row r="32" spans="1:68" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
+    <row r="32" spans="1:68" s="61" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="63">
         <v>45002.345046296286</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="63">
         <v>45002.569745370369</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I32" s="3"/>
-      <c r="J32" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="K32" s="26"/>
-      <c r="L32" s="26"/>
-      <c r="M32" s="1" t="s">
+      <c r="F32" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="J32" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="K32" s="25"/>
+      <c r="L32" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="M32" s="46" t="s">
         <v>23</v>
       </c>
+      <c r="N32" s="60"/>
     </row>
     <row r="33" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D33" s="2">
@@ -2297,9 +2526,9 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="26"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
+      <c r="L33" s="46"/>
     </row>
     <row r="34" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D34" s="5">
@@ -2312,9 +2541,9 @@
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="27"/>
-      <c r="L34" s="27"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="26"/>
+      <c r="L34" s="48"/>
       <c r="M34" s="16"/>
       <c r="N34" s="20"/>
       <c r="O34"/>
@@ -2394,15 +2623,17 @@
       <c r="G35" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H35" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="I35" s="25"/>
-      <c r="J35" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="K35" s="28"/>
-      <c r="L35" s="28"/>
+      <c r="H35" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I35" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="J35" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="K35" s="27"/>
+      <c r="L35" s="45"/>
       <c r="M35" s="17"/>
       <c r="N35" s="20"/>
       <c r="O35"/>
@@ -2482,15 +2713,17 @@
       <c r="G36" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H36" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="I36" s="25"/>
-      <c r="J36" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="K36" s="26"/>
-      <c r="L36" s="26"/>
+      <c r="H36" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="J36" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="K36" s="25"/>
+      <c r="L36" s="46"/>
     </row>
     <row r="37" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D37" s="5">
@@ -2503,9 +2736,9 @@
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
-      <c r="J37" s="27"/>
-      <c r="K37" s="27"/>
-      <c r="L37" s="27"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="26"/>
+      <c r="L37" s="48"/>
       <c r="M37" s="16"/>
       <c r="N37" s="20"/>
       <c r="O37"/>
@@ -2588,12 +2821,14 @@
       <c r="H38" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I38" s="3"/>
-      <c r="J38" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="K38" s="26"/>
-      <c r="L38" s="26"/>
+      <c r="I38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J38" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="K38" s="25"/>
+      <c r="L38" s="46"/>
     </row>
     <row r="39" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D39" s="2">
@@ -2606,9 +2841,9 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
-      <c r="J39" s="26"/>
-      <c r="K39" s="26"/>
-      <c r="L39" s="26"/>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25"/>
+      <c r="L39" s="46"/>
     </row>
     <row r="40" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D40" s="2">
@@ -2621,9 +2856,9 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
-      <c r="J40" s="26"/>
-      <c r="K40" s="26"/>
-      <c r="L40" s="26"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="25"/>
+      <c r="L40" s="46"/>
     </row>
     <row r="41" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D41" s="2">
@@ -2636,9 +2871,9 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
-      <c r="J41" s="26"/>
-      <c r="K41" s="26"/>
-      <c r="L41" s="26"/>
+      <c r="J41" s="25"/>
+      <c r="K41" s="25"/>
+      <c r="L41" s="46"/>
     </row>
     <row r="42" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D42" s="5">
@@ -2651,9 +2886,9 @@
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
-      <c r="J42" s="27"/>
-      <c r="K42" s="27"/>
-      <c r="L42" s="27"/>
+      <c r="J42" s="26"/>
+      <c r="K42" s="26"/>
+      <c r="L42" s="48"/>
       <c r="M42" s="16"/>
       <c r="N42" s="20"/>
       <c r="O42"/>
@@ -2736,12 +2971,16 @@
       <c r="H43" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="9"/>
-      <c r="J43" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="K43" s="28"/>
-      <c r="L43" s="28"/>
+      <c r="I43" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J43" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="K43" s="27"/>
+      <c r="L43" s="45" t="s">
+        <v>57</v>
+      </c>
       <c r="M43" s="17" t="s">
         <v>50</v>
       </c>
@@ -2826,12 +3065,14 @@
       <c r="H44" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I44" s="3"/>
-      <c r="J44" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="K44" s="26"/>
-      <c r="L44" s="26"/>
+      <c r="I44" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J44" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="K44" s="25"/>
+      <c r="L44" s="46"/>
     </row>
     <row r="45" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D45" s="2">
@@ -2844,9 +3085,9 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
-      <c r="J45" s="26"/>
-      <c r="K45" s="26"/>
-      <c r="L45" s="26"/>
+      <c r="J45" s="25"/>
+      <c r="K45" s="25"/>
+      <c r="L45" s="46"/>
     </row>
     <row r="46" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D46" s="5">
@@ -2859,9 +3100,9 @@
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
-      <c r="J46" s="27"/>
-      <c r="K46" s="27"/>
-      <c r="L46" s="27"/>
+      <c r="J46" s="26"/>
+      <c r="K46" s="26"/>
+      <c r="L46" s="48"/>
       <c r="M46" s="16"/>
       <c r="N46" s="20"/>
       <c r="O46"/>
@@ -2944,12 +3185,16 @@
       <c r="H47" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I47" s="9"/>
-      <c r="J47" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="K47" s="28"/>
-      <c r="L47" s="28"/>
+      <c r="I47" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J47" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="K47" s="27"/>
+      <c r="L47" s="45" t="s">
+        <v>61</v>
+      </c>
       <c r="M47" s="17"/>
       <c r="N47" s="20"/>
       <c r="O47"/>
@@ -3032,12 +3277,16 @@
       <c r="H48" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I48" s="3"/>
-      <c r="J48" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="K48" s="26"/>
-      <c r="L48" s="26"/>
+      <c r="I48" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J48" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="K48" s="25"/>
+      <c r="L48" s="46" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="49" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D49" s="5">
@@ -3050,9 +3299,9 @@
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
-      <c r="J49" s="27"/>
-      <c r="K49" s="27"/>
-      <c r="L49" s="27"/>
+      <c r="J49" s="26"/>
+      <c r="K49" s="26"/>
+      <c r="L49" s="48"/>
       <c r="M49" s="16"/>
       <c r="N49" s="20"/>
       <c r="O49"/>
@@ -3135,12 +3384,14 @@
       <c r="H50" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I50" s="9"/>
-      <c r="J50" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="K50" s="28"/>
-      <c r="L50" s="28"/>
+      <c r="I50" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J50" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="K50" s="27"/>
+      <c r="L50" s="45"/>
       <c r="M50" s="17"/>
       <c r="N50" s="20"/>
       <c r="O50"/>
@@ -3223,12 +3474,14 @@
       <c r="H51" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I51" s="12"/>
-      <c r="J51" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="K51" s="29"/>
-      <c r="L51" s="29"/>
+      <c r="I51" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J51" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K51" s="28"/>
+      <c r="L51" s="51"/>
       <c r="M51" s="18"/>
       <c r="N51" s="20"/>
       <c r="O51"/>
@@ -3286,186 +3539,199 @@
       <c r="BO51"/>
       <c r="BP51"/>
     </row>
-    <row r="52" spans="1:68" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
+    <row r="52" spans="1:68" s="33" customFormat="1" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="B52" s="24" t="s">
+      <c r="B52" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="C52" s="24" t="s">
+      <c r="C52" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="D52" s="2">
+      <c r="D52" s="34">
         <v>42612.580873842591</v>
       </c>
-      <c r="E52" s="2">
+      <c r="E52" s="34">
         <v>42612.603443287036</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="F52" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="G52" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="H52" s="3" t="s">
+      <c r="H52" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="I52" s="3"/>
-      <c r="J52" s="26" t="s">
+      <c r="I52" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K52" s="26"/>
-      <c r="L52" s="26"/>
-      <c r="M52" s="31" t="s">
+      <c r="J52" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="K52" s="36"/>
+      <c r="L52" s="49"/>
+      <c r="M52" s="37" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="53" spans="1:68" x14ac:dyDescent="0.45">
-      <c r="D53" s="2">
+      <c r="N52" s="38"/>
+    </row>
+    <row r="53" spans="1:68" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D53" s="34">
         <v>42614.355943287039</v>
       </c>
-      <c r="E53" s="2">
+      <c r="E53" s="34">
         <v>42614.377528935191</v>
       </c>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="26"/>
-      <c r="K53" s="26"/>
-      <c r="L53" s="26"/>
-    </row>
-    <row r="54" spans="1:68" x14ac:dyDescent="0.45">
-      <c r="D54" s="2">
+      <c r="F53" s="35"/>
+      <c r="G53" s="35"/>
+      <c r="H53" s="35"/>
+      <c r="I53" s="35"/>
+      <c r="J53" s="36"/>
+      <c r="K53" s="36"/>
+      <c r="L53" s="49"/>
+      <c r="M53" s="37"/>
+      <c r="N53" s="38"/>
+    </row>
+    <row r="54" spans="1:68" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D54" s="34">
         <v>42615.103859953699</v>
       </c>
-      <c r="E54" s="2">
+      <c r="E54" s="34">
         <v>42615.120468749999</v>
       </c>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-      <c r="J54" s="26"/>
-      <c r="K54" s="26"/>
-      <c r="L54" s="26"/>
-    </row>
-    <row r="55" spans="1:68" x14ac:dyDescent="0.45">
-      <c r="D55" s="2">
+      <c r="F54" s="35"/>
+      <c r="G54" s="35"/>
+      <c r="H54" s="35"/>
+      <c r="I54" s="35"/>
+      <c r="J54" s="36"/>
+      <c r="K54" s="36"/>
+      <c r="L54" s="49"/>
+      <c r="M54" s="37"/>
+      <c r="N54" s="38"/>
+    </row>
+    <row r="55" spans="1:68" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D55" s="34">
         <v>42616.176603009248</v>
       </c>
-      <c r="E55" s="2">
+      <c r="E55" s="34">
         <v>42616.210109953703</v>
       </c>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="26"/>
-      <c r="K55" s="26"/>
-      <c r="L55" s="26"/>
-    </row>
-    <row r="56" spans="1:68" x14ac:dyDescent="0.45">
-      <c r="D56" s="2">
+      <c r="F55" s="35"/>
+      <c r="G55" s="35"/>
+      <c r="H55" s="35"/>
+      <c r="I55" s="35"/>
+      <c r="J55" s="36"/>
+      <c r="K55" s="36"/>
+      <c r="L55" s="49"/>
+      <c r="M55" s="37"/>
+      <c r="N55" s="38"/>
+    </row>
+    <row r="56" spans="1:68" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D56" s="34">
         <v>42616.414797453697</v>
       </c>
-      <c r="E56" s="2">
+      <c r="E56" s="34">
         <v>42616.434068287039</v>
       </c>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
-      <c r="J56" s="26"/>
-      <c r="K56" s="26"/>
-      <c r="L56" s="26"/>
-    </row>
-    <row r="57" spans="1:68" x14ac:dyDescent="0.45">
-      <c r="D57" s="2">
+      <c r="F56" s="35"/>
+      <c r="G56" s="35"/>
+      <c r="H56" s="35"/>
+      <c r="I56" s="35"/>
+      <c r="J56" s="36"/>
+      <c r="K56" s="36"/>
+      <c r="L56" s="49"/>
+      <c r="M56" s="37"/>
+      <c r="N56" s="38"/>
+    </row>
+    <row r="57" spans="1:68" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D57" s="34">
         <v>42618.576927083333</v>
       </c>
-      <c r="E57" s="2">
+      <c r="E57" s="34">
         <v>42618.598454861123</v>
       </c>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
-      <c r="J57" s="26"/>
-      <c r="K57" s="26"/>
-      <c r="L57" s="26"/>
-    </row>
-    <row r="58" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="D58" s="5">
+      <c r="F57" s="35"/>
+      <c r="G57" s="35"/>
+      <c r="H57" s="35"/>
+      <c r="I57" s="35"/>
+      <c r="J57" s="36"/>
+      <c r="K57" s="36"/>
+      <c r="L57" s="49"/>
+      <c r="M57" s="37"/>
+      <c r="N57" s="38"/>
+    </row>
+    <row r="58" spans="1:68" s="39" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D58" s="40">
         <v>42623.506336805563</v>
       </c>
-      <c r="E58" s="5">
+      <c r="E58" s="40">
         <v>42623.522656250003</v>
       </c>
-      <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
-      <c r="H58" s="6"/>
-      <c r="I58" s="6"/>
-      <c r="J58" s="27"/>
-      <c r="K58" s="27"/>
-      <c r="L58" s="27"/>
-      <c r="M58" s="16"/>
-      <c r="N58" s="20"/>
-      <c r="O58"/>
-      <c r="P58"/>
-      <c r="Q58"/>
-      <c r="R58"/>
-      <c r="S58"/>
-      <c r="T58"/>
-      <c r="U58"/>
-      <c r="V58"/>
-      <c r="W58"/>
-      <c r="X58"/>
-      <c r="Y58"/>
-      <c r="Z58"/>
-      <c r="AA58"/>
-      <c r="AB58"/>
-      <c r="AC58"/>
-      <c r="AD58"/>
-      <c r="AE58"/>
-      <c r="AF58"/>
-      <c r="AG58"/>
-      <c r="AH58"/>
-      <c r="AI58"/>
-      <c r="AJ58"/>
-      <c r="AK58"/>
-      <c r="AL58"/>
-      <c r="AM58"/>
-      <c r="AN58"/>
-      <c r="AO58"/>
-      <c r="AP58"/>
-      <c r="AQ58"/>
-      <c r="AR58"/>
-      <c r="AS58"/>
-      <c r="AT58"/>
-      <c r="AU58"/>
-      <c r="AV58"/>
-      <c r="AW58"/>
-      <c r="AX58"/>
-      <c r="AY58"/>
-      <c r="AZ58"/>
-      <c r="BA58"/>
-      <c r="BB58"/>
-      <c r="BC58"/>
-      <c r="BD58"/>
-      <c r="BE58"/>
-      <c r="BF58"/>
-      <c r="BG58"/>
-      <c r="BH58"/>
-      <c r="BI58"/>
-      <c r="BJ58"/>
-      <c r="BK58"/>
-      <c r="BL58"/>
-      <c r="BM58"/>
-      <c r="BN58"/>
-      <c r="BO58"/>
-      <c r="BP58"/>
+      <c r="F58" s="41"/>
+      <c r="G58" s="41"/>
+      <c r="H58" s="41"/>
+      <c r="I58" s="41"/>
+      <c r="J58" s="42"/>
+      <c r="K58" s="42"/>
+      <c r="L58" s="50"/>
+      <c r="M58" s="43"/>
+      <c r="N58" s="38"/>
+      <c r="O58" s="33"/>
+      <c r="P58" s="33"/>
+      <c r="Q58" s="33"/>
+      <c r="R58" s="33"/>
+      <c r="S58" s="33"/>
+      <c r="T58" s="33"/>
+      <c r="U58" s="33"/>
+      <c r="V58" s="33"/>
+      <c r="W58" s="33"/>
+      <c r="X58" s="33"/>
+      <c r="Y58" s="33"/>
+      <c r="Z58" s="33"/>
+      <c r="AA58" s="33"/>
+      <c r="AB58" s="33"/>
+      <c r="AC58" s="33"/>
+      <c r="AD58" s="33"/>
+      <c r="AE58" s="33"/>
+      <c r="AF58" s="33"/>
+      <c r="AG58" s="33"/>
+      <c r="AH58" s="33"/>
+      <c r="AI58" s="33"/>
+      <c r="AJ58" s="33"/>
+      <c r="AK58" s="33"/>
+      <c r="AL58" s="33"/>
+      <c r="AM58" s="33"/>
+      <c r="AN58" s="33"/>
+      <c r="AO58" s="33"/>
+      <c r="AP58" s="33"/>
+      <c r="AQ58" s="33"/>
+      <c r="AR58" s="33"/>
+      <c r="AS58" s="33"/>
+      <c r="AT58" s="33"/>
+      <c r="AU58" s="33"/>
+      <c r="AV58" s="33"/>
+      <c r="AW58" s="33"/>
+      <c r="AX58" s="33"/>
+      <c r="AY58" s="33"/>
+      <c r="AZ58" s="33"/>
+      <c r="BA58" s="33"/>
+      <c r="BB58" s="33"/>
+      <c r="BC58" s="33"/>
+      <c r="BD58" s="33"/>
+      <c r="BE58" s="33"/>
+      <c r="BF58" s="33"/>
+      <c r="BG58" s="33"/>
+      <c r="BH58" s="33"/>
+      <c r="BI58" s="33"/>
+      <c r="BJ58" s="33"/>
+      <c r="BK58" s="33"/>
+      <c r="BL58" s="33"/>
+      <c r="BM58" s="33"/>
+      <c r="BN58" s="33"/>
+      <c r="BO58" s="33"/>
+      <c r="BP58" s="33"/>
     </row>
     <row r="59" spans="1:68" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
@@ -3492,12 +3758,16 @@
       <c r="H59" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I59" s="3"/>
-      <c r="J59" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="K59" s="26"/>
-      <c r="L59" s="26"/>
+      <c r="I59" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J59" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="K59" s="25"/>
+      <c r="L59" s="46" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="60" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D60" s="2">
@@ -3510,9 +3780,9 @@
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
-      <c r="J60" s="26"/>
-      <c r="K60" s="26"/>
-      <c r="L60" s="26"/>
+      <c r="J60" s="25"/>
+      <c r="K60" s="25"/>
+      <c r="L60" s="46"/>
     </row>
     <row r="61" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D61" s="2">
@@ -3525,9 +3795,9 @@
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
-      <c r="J61" s="26"/>
-      <c r="K61" s="26"/>
-      <c r="L61" s="26"/>
+      <c r="J61" s="25"/>
+      <c r="K61" s="25"/>
+      <c r="L61" s="46"/>
     </row>
     <row r="62" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D62" s="2">
@@ -3540,9 +3810,9 @@
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
-      <c r="J62" s="26"/>
-      <c r="K62" s="26"/>
-      <c r="L62" s="26"/>
+      <c r="J62" s="25"/>
+      <c r="K62" s="25"/>
+      <c r="L62" s="46"/>
     </row>
     <row r="63" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D63" s="5">
@@ -3555,9 +3825,9 @@
       <c r="G63" s="6"/>
       <c r="H63" s="6"/>
       <c r="I63" s="6"/>
-      <c r="J63" s="27"/>
-      <c r="K63" s="27"/>
-      <c r="L63" s="27"/>
+      <c r="J63" s="26"/>
+      <c r="K63" s="26"/>
+      <c r="L63" s="48"/>
       <c r="M63" s="16"/>
       <c r="N63" s="20"/>
       <c r="O63"/>
@@ -3640,12 +3910,16 @@
       <c r="H64" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I64" s="3"/>
-      <c r="J64" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="K64" s="26"/>
-      <c r="L64" s="26"/>
+      <c r="I64" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J64" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="K64" s="25"/>
+      <c r="L64" s="46" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="65" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D65" s="2">
@@ -3658,9 +3932,9 @@
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
-      <c r="J65" s="26"/>
-      <c r="K65" s="26"/>
-      <c r="L65" s="26"/>
+      <c r="J65" s="25"/>
+      <c r="K65" s="25"/>
+      <c r="L65" s="46"/>
     </row>
     <row r="66" spans="1:68" x14ac:dyDescent="0.45">
       <c r="D66" s="2">
@@ -3673,9 +3947,9 @@
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
-      <c r="J66" s="26"/>
-      <c r="K66" s="26"/>
-      <c r="L66" s="26"/>
+      <c r="J66" s="25"/>
+      <c r="K66" s="25"/>
+      <c r="L66" s="46"/>
     </row>
     <row r="67" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D67" s="5">
@@ -3688,9 +3962,9 @@
       <c r="G67" s="6"/>
       <c r="H67" s="6"/>
       <c r="I67" s="6"/>
-      <c r="J67" s="27"/>
-      <c r="K67" s="27"/>
-      <c r="L67" s="27"/>
+      <c r="J67" s="26"/>
+      <c r="K67" s="26"/>
+      <c r="L67" s="48"/>
       <c r="M67" s="16"/>
       <c r="N67" s="20"/>
       <c r="O67"/>
@@ -3748,231 +4022,250 @@
       <c r="BO67"/>
       <c r="BP67"/>
     </row>
-    <row r="68" spans="1:68" x14ac:dyDescent="0.45">
-      <c r="A68" t="s">
+    <row r="68" spans="1:68" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A68" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="B68" s="24" t="s">
+      <c r="B68" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="C68" s="24" t="s">
+      <c r="C68" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="D68" s="2">
+      <c r="D68" s="34">
         <v>42610.535399305547</v>
       </c>
-      <c r="E68" s="2">
+      <c r="E68" s="34">
         <v>42610.555225694443</v>
       </c>
-      <c r="F68" s="3" t="s">
+      <c r="F68" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="G68" s="3" t="s">
+      <c r="G68" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="H68" s="3" t="s">
+      <c r="H68" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="I68" s="3"/>
-      <c r="J68" s="26" t="s">
+      <c r="I68" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K68" s="26"/>
-      <c r="L68" s="26"/>
-      <c r="M68" s="31" t="s">
+      <c r="J68" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="K68" s="55"/>
+      <c r="L68" s="49"/>
+      <c r="M68" s="37" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="69" spans="1:68" x14ac:dyDescent="0.45">
-      <c r="D69" s="2">
+      <c r="N68" s="38"/>
+    </row>
+    <row r="69" spans="1:68" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D69" s="34">
         <v>42612.31131365741</v>
       </c>
-      <c r="E69" s="2">
+      <c r="E69" s="34">
         <v>42612.336788194443</v>
       </c>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
-      <c r="H69" s="3"/>
-      <c r="I69" s="3"/>
-      <c r="J69" s="26"/>
-      <c r="K69" s="26"/>
-      <c r="L69" s="26"/>
-    </row>
-    <row r="70" spans="1:68" x14ac:dyDescent="0.45">
-      <c r="D70" s="2">
+      <c r="F69" s="54"/>
+      <c r="G69" s="54"/>
+      <c r="H69" s="54"/>
+      <c r="I69" s="54"/>
+      <c r="J69" s="55"/>
+      <c r="K69" s="55"/>
+      <c r="L69" s="49"/>
+      <c r="M69" s="37"/>
+      <c r="N69" s="38"/>
+    </row>
+    <row r="70" spans="1:68" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D70" s="34">
         <v>42612.969021990742</v>
       </c>
-      <c r="E70" s="2">
+      <c r="E70" s="34">
         <v>42612.983778935188</v>
       </c>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
-      <c r="I70" s="3"/>
-      <c r="J70" s="26"/>
-      <c r="K70" s="26"/>
-      <c r="L70" s="26"/>
-    </row>
-    <row r="71" spans="1:68" x14ac:dyDescent="0.45">
-      <c r="D71" s="2">
+      <c r="F70" s="54"/>
+      <c r="G70" s="54"/>
+      <c r="H70" s="54"/>
+      <c r="I70" s="54"/>
+      <c r="J70" s="55"/>
+      <c r="K70" s="55"/>
+      <c r="L70" s="49"/>
+      <c r="M70" s="37"/>
+      <c r="N70" s="38"/>
+    </row>
+    <row r="71" spans="1:68" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D71" s="34">
         <v>42616.257019675933</v>
       </c>
-      <c r="E71" s="2">
+      <c r="E71" s="34">
         <v>42616.291394675922</v>
       </c>
-      <c r="F71" s="3"/>
-      <c r="G71" s="3"/>
-      <c r="H71" s="3"/>
-      <c r="I71" s="3"/>
-      <c r="J71" s="26"/>
-      <c r="K71" s="26"/>
-      <c r="L71" s="26"/>
-    </row>
-    <row r="72" spans="1:68" x14ac:dyDescent="0.45">
-      <c r="D72" s="2">
+      <c r="F71" s="54"/>
+      <c r="G71" s="54"/>
+      <c r="H71" s="54"/>
+      <c r="I71" s="54"/>
+      <c r="J71" s="55"/>
+      <c r="K71" s="55"/>
+      <c r="L71" s="49"/>
+      <c r="M71" s="37"/>
+      <c r="N71" s="38"/>
+    </row>
+    <row r="72" spans="1:68" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D72" s="34">
         <v>42621.241869212958</v>
       </c>
-      <c r="E72" s="2">
+      <c r="E72" s="34">
         <v>42621.275318287036</v>
       </c>
-      <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
-      <c r="H72" s="3"/>
-      <c r="I72" s="3"/>
-      <c r="J72" s="26"/>
-      <c r="K72" s="26"/>
-      <c r="L72" s="26"/>
-    </row>
-    <row r="73" spans="1:68" x14ac:dyDescent="0.45">
-      <c r="D73" s="2">
+      <c r="F72" s="54"/>
+      <c r="G72" s="54"/>
+      <c r="H72" s="54"/>
+      <c r="I72" s="54"/>
+      <c r="J72" s="55"/>
+      <c r="K72" s="55"/>
+      <c r="L72" s="49"/>
+      <c r="M72" s="37"/>
+      <c r="N72" s="38"/>
+    </row>
+    <row r="73" spans="1:68" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D73" s="34">
         <v>42623.419010416663</v>
       </c>
-      <c r="E73" s="2">
+      <c r="E73" s="34">
         <v>42623.431278935182</v>
       </c>
-      <c r="F73" s="3"/>
-      <c r="G73" s="3"/>
-      <c r="H73" s="3"/>
-      <c r="I73" s="3"/>
-      <c r="J73" s="26"/>
-      <c r="K73" s="26"/>
-      <c r="L73" s="26"/>
-    </row>
-    <row r="74" spans="1:68" x14ac:dyDescent="0.45">
-      <c r="D74" s="2">
+      <c r="F73" s="54"/>
+      <c r="G73" s="54"/>
+      <c r="H73" s="54"/>
+      <c r="I73" s="54"/>
+      <c r="J73" s="55"/>
+      <c r="K73" s="55"/>
+      <c r="L73" s="49"/>
+      <c r="M73" s="37"/>
+      <c r="N73" s="38"/>
+    </row>
+    <row r="74" spans="1:68" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D74" s="34">
         <v>42624.161082175917</v>
       </c>
-      <c r="E74" s="2">
+      <c r="E74" s="34">
         <v>42624.177401620371</v>
       </c>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
-      <c r="H74" s="3"/>
-      <c r="I74" s="3"/>
-      <c r="J74" s="26"/>
-      <c r="K74" s="26"/>
-      <c r="L74" s="26"/>
-    </row>
-    <row r="75" spans="1:68" x14ac:dyDescent="0.45">
-      <c r="D75" s="2">
+      <c r="F74" s="54"/>
+      <c r="G74" s="54"/>
+      <c r="H74" s="54"/>
+      <c r="I74" s="54"/>
+      <c r="J74" s="55"/>
+      <c r="K74" s="55"/>
+      <c r="L74" s="49"/>
+      <c r="M74" s="37"/>
+      <c r="N74" s="38"/>
+    </row>
+    <row r="75" spans="1:68" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D75" s="34">
         <v>42626.26449652778</v>
       </c>
-      <c r="E75" s="2">
+      <c r="E75" s="34">
         <v>42626.29942708333</v>
       </c>
-      <c r="F75" s="3"/>
-      <c r="G75" s="3"/>
-      <c r="H75" s="3"/>
-      <c r="I75" s="3"/>
-      <c r="J75" s="26"/>
-      <c r="K75" s="26"/>
-      <c r="L75" s="26"/>
-    </row>
-    <row r="76" spans="1:68" x14ac:dyDescent="0.45">
-      <c r="D76" s="2">
+      <c r="F75" s="54"/>
+      <c r="G75" s="54"/>
+      <c r="H75" s="54"/>
+      <c r="I75" s="54"/>
+      <c r="J75" s="55"/>
+      <c r="K75" s="55"/>
+      <c r="L75" s="49"/>
+      <c r="M75" s="37"/>
+      <c r="N75" s="38"/>
+    </row>
+    <row r="76" spans="1:68" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D76" s="34">
         <v>42626.344184027781</v>
       </c>
-      <c r="E76" s="2">
+      <c r="E76" s="34">
         <v>42626.386487268523</v>
       </c>
-      <c r="F76" s="3"/>
-      <c r="G76" s="3"/>
-      <c r="H76" s="3"/>
-      <c r="I76" s="3"/>
-      <c r="J76" s="26"/>
-      <c r="K76" s="26"/>
-      <c r="L76" s="26"/>
-    </row>
-    <row r="77" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="D77" s="5">
+      <c r="F76" s="54"/>
+      <c r="G76" s="54"/>
+      <c r="H76" s="54"/>
+      <c r="I76" s="54"/>
+      <c r="J76" s="55"/>
+      <c r="K76" s="55"/>
+      <c r="L76" s="49"/>
+      <c r="M76" s="37"/>
+      <c r="N76" s="38"/>
+    </row>
+    <row r="77" spans="1:68" s="39" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D77" s="40">
         <v>42627.304484953696</v>
       </c>
-      <c r="E77" s="5">
+      <c r="E77" s="40">
         <v>42627.315017361107</v>
       </c>
-      <c r="F77" s="6"/>
-      <c r="G77" s="6"/>
-      <c r="H77" s="6"/>
-      <c r="I77" s="6"/>
-      <c r="J77" s="27"/>
-      <c r="K77" s="27"/>
-      <c r="L77" s="27"/>
-      <c r="M77" s="16"/>
-      <c r="N77" s="20"/>
-      <c r="O77"/>
-      <c r="P77"/>
-      <c r="Q77"/>
-      <c r="R77"/>
-      <c r="S77"/>
-      <c r="T77"/>
-      <c r="U77"/>
-      <c r="V77"/>
-      <c r="W77"/>
-      <c r="X77"/>
-      <c r="Y77"/>
-      <c r="Z77"/>
-      <c r="AA77"/>
-      <c r="AB77"/>
-      <c r="AC77"/>
-      <c r="AD77"/>
-      <c r="AE77"/>
-      <c r="AF77"/>
-      <c r="AG77"/>
-      <c r="AH77"/>
-      <c r="AI77"/>
-      <c r="AJ77"/>
-      <c r="AK77"/>
-      <c r="AL77"/>
-      <c r="AM77"/>
-      <c r="AN77"/>
-      <c r="AO77"/>
-      <c r="AP77"/>
-      <c r="AQ77"/>
-      <c r="AR77"/>
-      <c r="AS77"/>
-      <c r="AT77"/>
-      <c r="AU77"/>
-      <c r="AV77"/>
-      <c r="AW77"/>
-      <c r="AX77"/>
-      <c r="AY77"/>
-      <c r="AZ77"/>
-      <c r="BA77"/>
-      <c r="BB77"/>
-      <c r="BC77"/>
-      <c r="BD77"/>
-      <c r="BE77"/>
-      <c r="BF77"/>
-      <c r="BG77"/>
-      <c r="BH77"/>
-      <c r="BI77"/>
-      <c r="BJ77"/>
-      <c r="BK77"/>
-      <c r="BL77"/>
-      <c r="BM77"/>
-      <c r="BN77"/>
-      <c r="BO77"/>
-      <c r="BP77"/>
+      <c r="F77" s="56"/>
+      <c r="G77" s="56"/>
+      <c r="H77" s="56"/>
+      <c r="I77" s="56"/>
+      <c r="J77" s="57"/>
+      <c r="K77" s="57"/>
+      <c r="L77" s="50"/>
+      <c r="M77" s="43"/>
+      <c r="N77" s="38"/>
+      <c r="O77" s="33"/>
+      <c r="P77" s="33"/>
+      <c r="Q77" s="33"/>
+      <c r="R77" s="33"/>
+      <c r="S77" s="33"/>
+      <c r="T77" s="33"/>
+      <c r="U77" s="33"/>
+      <c r="V77" s="33"/>
+      <c r="W77" s="33"/>
+      <c r="X77" s="33"/>
+      <c r="Y77" s="33"/>
+      <c r="Z77" s="33"/>
+      <c r="AA77" s="33"/>
+      <c r="AB77" s="33"/>
+      <c r="AC77" s="33"/>
+      <c r="AD77" s="33"/>
+      <c r="AE77" s="33"/>
+      <c r="AF77" s="33"/>
+      <c r="AG77" s="33"/>
+      <c r="AH77" s="33"/>
+      <c r="AI77" s="33"/>
+      <c r="AJ77" s="33"/>
+      <c r="AK77" s="33"/>
+      <c r="AL77" s="33"/>
+      <c r="AM77" s="33"/>
+      <c r="AN77" s="33"/>
+      <c r="AO77" s="33"/>
+      <c r="AP77" s="33"/>
+      <c r="AQ77" s="33"/>
+      <c r="AR77" s="33"/>
+      <c r="AS77" s="33"/>
+      <c r="AT77" s="33"/>
+      <c r="AU77" s="33"/>
+      <c r="AV77" s="33"/>
+      <c r="AW77" s="33"/>
+      <c r="AX77" s="33"/>
+      <c r="AY77" s="33"/>
+      <c r="AZ77" s="33"/>
+      <c r="BA77" s="33"/>
+      <c r="BB77" s="33"/>
+      <c r="BC77" s="33"/>
+      <c r="BD77" s="33"/>
+      <c r="BE77" s="33"/>
+      <c r="BF77" s="33"/>
+      <c r="BG77" s="33"/>
+      <c r="BH77" s="33"/>
+      <c r="BI77" s="33"/>
+      <c r="BJ77" s="33"/>
+      <c r="BK77" s="33"/>
+      <c r="BL77" s="33"/>
+      <c r="BM77" s="33"/>
+      <c r="BN77" s="33"/>
+      <c r="BO77" s="33"/>
+      <c r="BP77" s="33"/>
     </row>
     <row r="78" spans="1:68" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
@@ -3999,12 +4292,16 @@
       <c r="H78" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I78" s="3"/>
-      <c r="J78" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="K78" s="26"/>
-      <c r="L78" s="26"/>
+      <c r="I78" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J78" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="K78" s="25"/>
+      <c r="L78" s="46" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="79" spans="1:68" s="13" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D79" s="14">
@@ -4017,9 +4314,9 @@
       <c r="G79" s="15"/>
       <c r="H79" s="15"/>
       <c r="I79" s="15"/>
-      <c r="J79" s="30"/>
-      <c r="K79" s="30"/>
-      <c r="L79" s="30"/>
+      <c r="J79" s="29"/>
+      <c r="K79" s="29"/>
+      <c r="L79" s="52"/>
       <c r="M79" s="19"/>
       <c r="N79" s="20"/>
       <c r="O79"/>
@@ -4099,12 +4396,16 @@
       <c r="H80" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I80" s="3"/>
-      <c r="J80" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="K80" s="26"/>
-      <c r="L80" s="26"/>
+      <c r="I80" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J80" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="K80" s="25"/>
+      <c r="L80" s="46" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D81" s="2">
@@ -4114,9 +4415,9 @@
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
-      <c r="J81" s="26"/>
-      <c r="K81" s="26"/>
-      <c r="L81" s="26"/>
+      <c r="J81" s="25"/>
+      <c r="K81" s="25"/>
+      <c r="L81" s="46"/>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D82" s="2">
@@ -4126,9 +4427,9 @@
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
-      <c r="J82" s="26"/>
-      <c r="K82" s="26"/>
-      <c r="L82" s="26"/>
+      <c r="J82" s="25"/>
+      <c r="K82" s="25"/>
+      <c r="L82" s="46"/>
     </row>
     <row r="83" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D83" s="5">
@@ -4138,40 +4439,44 @@
       <c r="G83" s="6"/>
       <c r="H83" s="6"/>
       <c r="I83" s="6"/>
-      <c r="J83" s="27"/>
-      <c r="K83" s="27"/>
-      <c r="L83" s="27"/>
+      <c r="J83" s="26"/>
+      <c r="K83" s="26"/>
+      <c r="L83" s="48"/>
       <c r="M83" s="16"/>
       <c r="N83" s="22"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A84" t="s">
+    <row r="84" spans="1:14" s="61" customFormat="1" ht="57.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A84" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="D84" s="2">
+      <c r="D84" s="63">
         <v>43338.193535879633</v>
       </c>
-      <c r="F84" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H84" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I84" s="3"/>
-      <c r="J84" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="K84" s="26"/>
-      <c r="L84" s="26"/>
+      <c r="F84" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G84" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="H84" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="I84" s="25"/>
+      <c r="J84" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="K84" s="25"/>
+      <c r="L84" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="M84" s="46"/>
+      <c r="N84" s="60"/>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D85" s="2">
@@ -4181,9 +4486,9 @@
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
-      <c r="J85" s="26"/>
-      <c r="K85" s="26"/>
-      <c r="L85" s="26"/>
+      <c r="J85" s="25"/>
+      <c r="K85" s="25"/>
+      <c r="L85" s="46"/>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D86" s="2">
@@ -4193,9 +4498,9 @@
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
-      <c r="J86" s="26"/>
-      <c r="K86" s="26"/>
-      <c r="L86" s="26"/>
+      <c r="J86" s="25"/>
+      <c r="K86" s="25"/>
+      <c r="L86" s="46"/>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D87" s="2">
@@ -4205,9 +4510,9 @@
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
-      <c r="J87" s="26"/>
-      <c r="K87" s="26"/>
-      <c r="L87" s="26"/>
+      <c r="J87" s="25"/>
+      <c r="K87" s="25"/>
+      <c r="L87" s="46"/>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D88" s="2">
@@ -4217,9 +4522,9 @@
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
-      <c r="J88" s="26"/>
-      <c r="K88" s="26"/>
-      <c r="L88" s="26"/>
+      <c r="J88" s="25"/>
+      <c r="K88" s="25"/>
+      <c r="L88" s="46"/>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D89" s="2">
@@ -4229,9 +4534,9 @@
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
-      <c r="J89" s="26"/>
-      <c r="K89" s="26"/>
-      <c r="L89" s="26"/>
+      <c r="J89" s="25"/>
+      <c r="K89" s="25"/>
+      <c r="L89" s="46"/>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D90" s="2">
@@ -4241,9 +4546,9 @@
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
-      <c r="J90" s="26"/>
-      <c r="K90" s="26"/>
-      <c r="L90" s="26"/>
+      <c r="J90" s="25"/>
+      <c r="K90" s="25"/>
+      <c r="L90" s="46"/>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D91" s="2">
@@ -4253,9 +4558,9 @@
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
-      <c r="J91" s="26"/>
-      <c r="K91" s="26"/>
-      <c r="L91" s="26"/>
+      <c r="J91" s="25"/>
+      <c r="K91" s="25"/>
+      <c r="L91" s="46"/>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D92" s="2">
@@ -4265,9 +4570,9 @@
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
-      <c r="J92" s="26"/>
-      <c r="K92" s="26"/>
-      <c r="L92" s="26"/>
+      <c r="J92" s="25"/>
+      <c r="K92" s="25"/>
+      <c r="L92" s="46"/>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D93" s="2">
@@ -4277,9 +4582,9 @@
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
-      <c r="J93" s="26"/>
-      <c r="K93" s="26"/>
-      <c r="L93" s="26"/>
+      <c r="J93" s="25"/>
+      <c r="K93" s="25"/>
+      <c r="L93" s="46"/>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D94" s="2">
@@ -4289,9 +4594,9 @@
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
-      <c r="J94" s="26"/>
-      <c r="K94" s="26"/>
-      <c r="L94" s="26"/>
+      <c r="J94" s="25"/>
+      <c r="K94" s="25"/>
+      <c r="L94" s="46"/>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D95" s="2">
@@ -4301,9 +4606,9 @@
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
-      <c r="J95" s="26"/>
-      <c r="K95" s="26"/>
-      <c r="L95" s="26"/>
+      <c r="J95" s="25"/>
+      <c r="K95" s="25"/>
+      <c r="L95" s="46"/>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D96" s="2">
@@ -4313,9 +4618,9 @@
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
-      <c r="J96" s="26"/>
-      <c r="K96" s="26"/>
-      <c r="L96" s="26"/>
+      <c r="J96" s="25"/>
+      <c r="K96" s="25"/>
+      <c r="L96" s="46"/>
     </row>
     <row r="97" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D97" s="2">
@@ -4325,9 +4630,9 @@
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
-      <c r="J97" s="26"/>
-      <c r="K97" s="26"/>
-      <c r="L97" s="26"/>
+      <c r="J97" s="25"/>
+      <c r="K97" s="25"/>
+      <c r="L97" s="46"/>
     </row>
     <row r="98" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D98" s="2">
@@ -4337,9 +4642,9 @@
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
-      <c r="J98" s="26"/>
-      <c r="K98" s="26"/>
-      <c r="L98" s="26"/>
+      <c r="J98" s="25"/>
+      <c r="K98" s="25"/>
+      <c r="L98" s="46"/>
     </row>
     <row r="99" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D99" s="2">
@@ -4349,9 +4654,9 @@
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
-      <c r="J99" s="26"/>
-      <c r="K99" s="26"/>
-      <c r="L99" s="26"/>
+      <c r="J99" s="25"/>
+      <c r="K99" s="25"/>
+      <c r="L99" s="46"/>
     </row>
     <row r="100" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D100" s="2">
@@ -4361,9 +4666,9 @@
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
-      <c r="J100" s="26"/>
-      <c r="K100" s="26"/>
-      <c r="L100" s="26"/>
+      <c r="J100" s="25"/>
+      <c r="K100" s="25"/>
+      <c r="L100" s="46"/>
     </row>
     <row r="101" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D101" s="2">
@@ -4373,9 +4678,9 @@
       <c r="G101" s="3"/>
       <c r="H101" s="3"/>
       <c r="I101" s="3"/>
-      <c r="J101" s="26"/>
-      <c r="K101" s="26"/>
-      <c r="L101" s="26"/>
+      <c r="J101" s="25"/>
+      <c r="K101" s="25"/>
+      <c r="L101" s="46"/>
     </row>
     <row r="102" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D102" s="2">
@@ -4385,9 +4690,9 @@
       <c r="G102" s="3"/>
       <c r="H102" s="3"/>
       <c r="I102" s="3"/>
-      <c r="J102" s="26"/>
-      <c r="K102" s="26"/>
-      <c r="L102" s="26"/>
+      <c r="J102" s="25"/>
+      <c r="K102" s="25"/>
+      <c r="L102" s="46"/>
     </row>
     <row r="103" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D103" s="2">
@@ -4397,9 +4702,9 @@
       <c r="G103" s="3"/>
       <c r="H103" s="3"/>
       <c r="I103" s="3"/>
-      <c r="J103" s="26"/>
-      <c r="K103" s="26"/>
-      <c r="L103" s="26"/>
+      <c r="J103" s="25"/>
+      <c r="K103" s="25"/>
+      <c r="L103" s="46"/>
     </row>
     <row r="104" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D104" s="2">
@@ -4409,9 +4714,9 @@
       <c r="G104" s="3"/>
       <c r="H104" s="3"/>
       <c r="I104" s="3"/>
-      <c r="J104" s="26"/>
-      <c r="K104" s="26"/>
-      <c r="L104" s="26"/>
+      <c r="J104" s="25"/>
+      <c r="K104" s="25"/>
+      <c r="L104" s="46"/>
     </row>
     <row r="105" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D105" s="2">
@@ -4421,9 +4726,9 @@
       <c r="G105" s="3"/>
       <c r="H105" s="3"/>
       <c r="I105" s="3"/>
-      <c r="J105" s="26"/>
-      <c r="K105" s="26"/>
-      <c r="L105" s="26"/>
+      <c r="J105" s="25"/>
+      <c r="K105" s="25"/>
+      <c r="L105" s="46"/>
     </row>
     <row r="106" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D106" s="2">
@@ -4433,9 +4738,9 @@
       <c r="G106" s="3"/>
       <c r="H106" s="3"/>
       <c r="I106" s="3"/>
-      <c r="J106" s="26"/>
-      <c r="K106" s="26"/>
-      <c r="L106" s="26"/>
+      <c r="J106" s="25"/>
+      <c r="K106" s="25"/>
+      <c r="L106" s="46"/>
     </row>
     <row r="107" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D107" s="2">
@@ -4445,9 +4750,9 @@
       <c r="G107" s="3"/>
       <c r="H107" s="3"/>
       <c r="I107" s="3"/>
-      <c r="J107" s="26"/>
-      <c r="K107" s="26"/>
-      <c r="L107" s="26"/>
+      <c r="J107" s="25"/>
+      <c r="K107" s="25"/>
+      <c r="L107" s="46"/>
     </row>
     <row r="108" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D108" s="2">
@@ -4457,9 +4762,9 @@
       <c r="G108" s="3"/>
       <c r="H108" s="3"/>
       <c r="I108" s="3"/>
-      <c r="J108" s="26"/>
-      <c r="K108" s="26"/>
-      <c r="L108" s="26"/>
+      <c r="J108" s="25"/>
+      <c r="K108" s="25"/>
+      <c r="L108" s="46"/>
     </row>
     <row r="109" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D109" s="2">
@@ -4469,9 +4774,9 @@
       <c r="G109" s="3"/>
       <c r="H109" s="3"/>
       <c r="I109" s="3"/>
-      <c r="J109" s="26"/>
-      <c r="K109" s="26"/>
-      <c r="L109" s="26"/>
+      <c r="J109" s="25"/>
+      <c r="K109" s="25"/>
+      <c r="L109" s="46"/>
     </row>
     <row r="110" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D110" s="2">
@@ -4481,9 +4786,9 @@
       <c r="G110" s="3"/>
       <c r="H110" s="3"/>
       <c r="I110" s="3"/>
-      <c r="J110" s="26"/>
-      <c r="K110" s="26"/>
-      <c r="L110" s="26"/>
+      <c r="J110" s="25"/>
+      <c r="K110" s="25"/>
+      <c r="L110" s="46"/>
     </row>
     <row r="111" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D111" s="2">
@@ -4493,9 +4798,9 @@
       <c r="G111" s="3"/>
       <c r="H111" s="3"/>
       <c r="I111" s="3"/>
-      <c r="J111" s="26"/>
-      <c r="K111" s="26"/>
-      <c r="L111" s="26"/>
+      <c r="J111" s="25"/>
+      <c r="K111" s="25"/>
+      <c r="L111" s="46"/>
     </row>
     <row r="112" spans="4:12" x14ac:dyDescent="0.45">
       <c r="D112" s="2">
@@ -4505,9 +4810,9 @@
       <c r="G112" s="3"/>
       <c r="H112" s="3"/>
       <c r="I112" s="3"/>
-      <c r="J112" s="26"/>
-      <c r="K112" s="26"/>
-      <c r="L112" s="26"/>
+      <c r="J112" s="25"/>
+      <c r="K112" s="25"/>
+      <c r="L112" s="46"/>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D113" s="2">
@@ -4517,9 +4822,9 @@
       <c r="G113" s="3"/>
       <c r="H113" s="3"/>
       <c r="I113" s="3"/>
-      <c r="J113" s="26"/>
-      <c r="K113" s="26"/>
-      <c r="L113" s="26"/>
+      <c r="J113" s="25"/>
+      <c r="K113" s="25"/>
+      <c r="L113" s="46"/>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D114" s="2">
@@ -4529,9 +4834,9 @@
       <c r="G114" s="3"/>
       <c r="H114" s="3"/>
       <c r="I114" s="3"/>
-      <c r="J114" s="26"/>
-      <c r="K114" s="26"/>
-      <c r="L114" s="26"/>
+      <c r="J114" s="25"/>
+      <c r="K114" s="25"/>
+      <c r="L114" s="46"/>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D115" s="2">
@@ -4541,9 +4846,9 @@
       <c r="G115" s="3"/>
       <c r="H115" s="3"/>
       <c r="I115" s="3"/>
-      <c r="J115" s="26"/>
-      <c r="K115" s="26"/>
-      <c r="L115" s="26"/>
+      <c r="J115" s="25"/>
+      <c r="K115" s="25"/>
+      <c r="L115" s="46"/>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D116" s="2">
@@ -4553,9 +4858,9 @@
       <c r="G116" s="3"/>
       <c r="H116" s="3"/>
       <c r="I116" s="3"/>
-      <c r="J116" s="26"/>
-      <c r="K116" s="26"/>
-      <c r="L116" s="26"/>
+      <c r="J116" s="25"/>
+      <c r="K116" s="25"/>
+      <c r="L116" s="46"/>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D117" s="2">
@@ -4565,9 +4870,9 @@
       <c r="G117" s="3"/>
       <c r="H117" s="3"/>
       <c r="I117" s="3"/>
-      <c r="J117" s="26"/>
-      <c r="K117" s="26"/>
-      <c r="L117" s="26"/>
+      <c r="J117" s="25"/>
+      <c r="K117" s="25"/>
+      <c r="L117" s="46"/>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D118" s="2">
@@ -4577,9 +4882,9 @@
       <c r="G118" s="3"/>
       <c r="H118" s="3"/>
       <c r="I118" s="3"/>
-      <c r="J118" s="26"/>
-      <c r="K118" s="26"/>
-      <c r="L118" s="26"/>
+      <c r="J118" s="25"/>
+      <c r="K118" s="25"/>
+      <c r="L118" s="46"/>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D119" s="2">
@@ -4589,9 +4894,9 @@
       <c r="G119" s="3"/>
       <c r="H119" s="3"/>
       <c r="I119" s="3"/>
-      <c r="J119" s="26"/>
-      <c r="K119" s="26"/>
-      <c r="L119" s="26"/>
+      <c r="J119" s="25"/>
+      <c r="K119" s="25"/>
+      <c r="L119" s="46"/>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D120" s="2">
@@ -4601,9 +4906,9 @@
       <c r="G120" s="3"/>
       <c r="H120" s="3"/>
       <c r="I120" s="3"/>
-      <c r="J120" s="26"/>
-      <c r="K120" s="26"/>
-      <c r="L120" s="26"/>
+      <c r="J120" s="25"/>
+      <c r="K120" s="25"/>
+      <c r="L120" s="46"/>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D121" s="2">
@@ -4613,9 +4918,9 @@
       <c r="G121" s="3"/>
       <c r="H121" s="3"/>
       <c r="I121" s="3"/>
-      <c r="J121" s="26"/>
-      <c r="K121" s="26"/>
-      <c r="L121" s="26"/>
+      <c r="J121" s="25"/>
+      <c r="K121" s="25"/>
+      <c r="L121" s="46"/>
     </row>
     <row r="122" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="D122" s="5">
@@ -4625,9 +4930,9 @@
       <c r="G122" s="6"/>
       <c r="H122" s="6"/>
       <c r="I122" s="6"/>
-      <c r="J122" s="27"/>
-      <c r="K122" s="27"/>
-      <c r="L122" s="27"/>
+      <c r="J122" s="26"/>
+      <c r="K122" s="26"/>
+      <c r="L122" s="48"/>
       <c r="M122" s="16"/>
       <c r="N122" s="22"/>
     </row>
@@ -4644,7 +4949,7 @@
       <c r="D123" s="8">
         <v>43353.138153935193</v>
       </c>
-      <c r="F123" s="25" t="s">
+      <c r="F123" s="24" t="s">
         <v>7</v>
       </c>
       <c r="G123" s="9" t="s">
@@ -4653,10 +4958,14 @@
       <c r="H123" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I123" s="9"/>
-      <c r="J123" s="28"/>
-      <c r="K123" s="28"/>
-      <c r="L123" s="28"/>
+      <c r="I123" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J123" s="27"/>
+      <c r="K123" s="27"/>
+      <c r="L123" s="45" t="s">
+        <v>56</v>
+      </c>
       <c r="M123" s="17"/>
       <c r="N123" s="23"/>
     </row>
@@ -4673,7 +4982,7 @@
       <c r="D124" s="2">
         <v>43369.178304398149</v>
       </c>
-      <c r="F124" s="25" t="s">
+      <c r="F124" s="24" t="s">
         <v>7</v>
       </c>
       <c r="G124" s="3" t="s">
@@ -4682,10 +4991,14 @@
       <c r="H124" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I124" s="3"/>
-      <c r="J124" s="26"/>
-      <c r="K124" s="26"/>
-      <c r="L124" s="26"/>
+      <c r="I124" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J124" s="25"/>
+      <c r="K124" s="25"/>
+      <c r="L124" s="46" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D125" s="2">
@@ -4695,9 +5008,9 @@
       <c r="G125" s="3"/>
       <c r="H125" s="3"/>
       <c r="I125" s="3"/>
-      <c r="J125" s="26"/>
-      <c r="K125" s="26"/>
-      <c r="L125" s="26"/>
+      <c r="J125" s="25"/>
+      <c r="K125" s="25"/>
+      <c r="L125" s="46"/>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D126" s="2">
@@ -4707,9 +5020,9 @@
       <c r="G126" s="3"/>
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
-      <c r="J126" s="26"/>
-      <c r="K126" s="26"/>
-      <c r="L126" s="26"/>
+      <c r="J126" s="25"/>
+      <c r="K126" s="25"/>
+      <c r="L126" s="46"/>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.45">
       <c r="D127" s="2">
@@ -4719,9 +5032,9 @@
       <c r="G127" s="3"/>
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
-      <c r="J127" s="26"/>
-      <c r="K127" s="26"/>
-      <c r="L127" s="26"/>
+      <c r="J127" s="25"/>
+      <c r="K127" s="25"/>
+      <c r="L127" s="46"/>
     </row>
     <row r="128" spans="1:14" s="13" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="D128" s="14">
@@ -4731,9 +5044,9 @@
       <c r="G128" s="15"/>
       <c r="H128" s="15"/>
       <c r="I128" s="15"/>
-      <c r="J128" s="30"/>
-      <c r="K128" s="30"/>
-      <c r="L128" s="30"/>
+      <c r="J128" s="29"/>
+      <c r="K128" s="29"/>
+      <c r="L128" s="52"/>
       <c r="M128" s="19"/>
       <c r="N128" s="21"/>
     </row>
@@ -4741,5 +5054,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Creation of Spectrograms and Spectra for Cleaned Databases
</commit_message>
<xml_diff>
--- a/Analysis_Progress.xlsx
+++ b/Analysis_Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9d4c4f1623d30376/Documents/GitHub/Rissos_Geographic_Variation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="769" documentId="8_{C4C2D1DD-6DD6-49C2-8C12-51DEE2FC981A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82B57E13-375B-4C2E-B3AD-E526B4386654}"/>
+  <xr:revisionPtr revIDLastSave="772" documentId="8_{C4C2D1DD-6DD6-49C2-8C12-51DEE2FC981A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECC24861-6228-4708-96EF-13DCAC91692A}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{8391C37B-1672-4229-8478-45F991E75901}"/>
+    <workbookView xWindow="8220" yWindow="338" windowWidth="10057" windowHeight="8677" xr2:uid="{8391C37B-1672-4229-8478-45F991E75901}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -294,13 +294,13 @@
     <t>***</t>
   </si>
   <si>
-    <t>*** Either vessel or dolphin noise - Risso's present when detections not listed?</t>
-  </si>
-  <si>
-    <t>***Very faint banding with background noise</t>
-  </si>
-  <si>
     <t>Not uing this drift</t>
+  </si>
+  <si>
+    <t>*** Detection 1 - a couple dark lines to remove, 2 - low clicks, 3 - mixed species encounter with Lags (do not use), 4 - ok but occurs right after Lag enocunter, 5 - mixed species encounter (do not use)</t>
+  </si>
+  <si>
+    <t>***Very faint banding meaning distant detection</t>
   </si>
 </sst>
 </file>
@@ -980,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A18B98B-9FEB-4551-88CC-94F33BC1EF6E}">
   <dimension ref="A1:BQ129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F24" zoomScale="48" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" topLeftCell="M33" zoomScale="82" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2213,7 +2213,7 @@
         <v>69</v>
       </c>
       <c r="M20" s="64" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>16</v>
@@ -3054,7 +3054,7 @@
         <v>57</v>
       </c>
       <c r="M43" s="65" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N43" s="17" t="s">
         <v>50</v>
@@ -3864,7 +3864,7 @@
         <v>73</v>
       </c>
       <c r="N59" s="37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O59" s="38"/>
     </row>

</xml_diff>

<commit_message>
Updates to Thesis Progress
</commit_message>
<xml_diff>
--- a/Analysis_Progress.xlsx
+++ b/Analysis_Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9d4c4f1623d30376/Documents/GitHub/Rissos_Geographic_Variation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1683" documentId="8_{C4C2D1DD-6DD6-49C2-8C12-51DEE2FC981A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10BB6CC1-ADE9-4A6B-ADCC-368DD2242D38}"/>
+  <xr:revisionPtr revIDLastSave="1882" documentId="8_{C4C2D1DD-6DD6-49C2-8C12-51DEE2FC981A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{763EA40C-9823-473B-BE4A-5D47A8B6D1FA}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{8391C37B-1672-4229-8478-45F991E75901}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="269">
   <si>
     <t>PG_Click_Detections</t>
   </si>
@@ -837,13 +837,13 @@
     <t>Come back to this later</t>
   </si>
   <si>
-    <t>Possible Mixed-Species encounter</t>
-  </si>
-  <si>
-    <t>Possible Mixed-Species encounter - has been cleaned (see spectrogram)</t>
-  </si>
-  <si>
-    <t>Cleaned - waiting on R to confirm</t>
+    <t>Not using this drift - Multi-species detection</t>
+  </si>
+  <si>
+    <t>Not using this dift - Multi-species detection</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1080,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1266,10 +1266,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1610,13 +1628,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A18B98B-9FEB-4551-88CC-94F33BC1EF6E}">
   <dimension ref="A1:BR129"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScale="82" zoomScaleNormal="45" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80:XFD80"/>
+    <sheetView topLeftCell="A49" zoomScale="57" zoomScaleNormal="45" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="18.46484375" style="14" customWidth="1"/>
+    <col min="1" max="1" width="18.46484375" style="51" customWidth="1"/>
+    <col min="2" max="2" width="18.46484375" style="14" customWidth="1"/>
     <col min="3" max="3" width="19.06640625" style="14" customWidth="1"/>
     <col min="4" max="4" width="29.19921875" style="14" customWidth="1"/>
     <col min="5" max="5" width="23" style="14" customWidth="1"/>
@@ -1631,7 +1650,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:70" s="23" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="73" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="20" t="s">
@@ -1679,7 +1698,7 @@
       <c r="P1" s="22"/>
     </row>
     <row r="2" spans="1:70" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="51" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="14" t="s">
@@ -1717,6 +1736,7 @@
       </c>
     </row>
     <row r="3" spans="1:70" s="24" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="74"/>
       <c r="B3" s="24" t="s">
         <v>63</v>
       </c>
@@ -1804,7 +1824,7 @@
       <c r="BR3" s="14"/>
     </row>
     <row r="4" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="64" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="11" t="s">
@@ -1902,7 +1922,7 @@
       <c r="BR4" s="14"/>
     </row>
     <row r="5" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="64" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="11" t="s">
@@ -1998,7 +2018,7 @@
       <c r="BR5" s="14"/>
     </row>
     <row r="6" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="51" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="26" t="s">
@@ -2042,6 +2062,7 @@
       <c r="P6" s="28"/>
     </row>
     <row r="7" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="51"/>
       <c r="B7" s="26" t="s">
         <v>69</v>
       </c>
@@ -2075,6 +2096,7 @@
       <c r="P7" s="28"/>
     </row>
     <row r="8" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="51"/>
       <c r="B8" s="26" t="s">
         <v>70</v>
       </c>
@@ -2108,6 +2130,7 @@
       <c r="P8" s="28"/>
     </row>
     <row r="9" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="51"/>
       <c r="B9" s="26" t="s">
         <v>71</v>
       </c>
@@ -2141,6 +2164,7 @@
       <c r="P9" s="28"/>
     </row>
     <row r="10" spans="1:70" s="29" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="74"/>
       <c r="B10" s="29" t="s">
         <v>72</v>
       </c>
@@ -2228,7 +2252,7 @@
       <c r="BR10" s="26"/>
     </row>
     <row r="11" spans="1:70" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="54" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -2272,6 +2296,7 @@
       </c>
     </row>
     <row r="12" spans="1:70" s="29" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="74"/>
       <c r="B12" s="29" t="s">
         <v>74</v>
       </c>
@@ -2360,104 +2385,106 @@
       <c r="BQ12" s="26"/>
       <c r="BR12" s="26"/>
     </row>
-    <row r="13" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="11" t="s">
+    <row r="13" spans="1:70" s="39" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="12">
+      <c r="D13" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="40">
         <v>44818.156134259261</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="40">
         <v>44818.174768518518</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14"/>
-      <c r="U13" s="14"/>
-      <c r="V13" s="14"/>
-      <c r="W13" s="14"/>
-      <c r="X13" s="14"/>
-      <c r="Y13" s="14"/>
-      <c r="Z13" s="14"/>
-      <c r="AA13" s="14"/>
-      <c r="AB13" s="14"/>
-      <c r="AC13" s="14"/>
-      <c r="AD13" s="14"/>
-      <c r="AE13" s="14"/>
-      <c r="AF13" s="14"/>
-      <c r="AG13" s="14"/>
-      <c r="AH13" s="14"/>
-      <c r="AI13" s="14"/>
-      <c r="AJ13" s="14"/>
-      <c r="AK13" s="14"/>
-      <c r="AL13" s="14"/>
-      <c r="AM13" s="14"/>
-      <c r="AN13" s="14"/>
-      <c r="AO13" s="14"/>
-      <c r="AP13" s="14"/>
-      <c r="AQ13" s="14"/>
-      <c r="AR13" s="14"/>
-      <c r="AS13" s="14"/>
-      <c r="AT13" s="14"/>
-      <c r="AU13" s="14"/>
-      <c r="AV13" s="14"/>
-      <c r="AW13" s="14"/>
-      <c r="AX13" s="14"/>
-      <c r="AY13" s="14"/>
-      <c r="AZ13" s="14"/>
-      <c r="BA13" s="14"/>
-      <c r="BB13" s="14"/>
-      <c r="BC13" s="14"/>
-      <c r="BD13" s="14"/>
-      <c r="BE13" s="14"/>
-      <c r="BF13" s="14"/>
-      <c r="BG13" s="14"/>
-      <c r="BH13" s="14"/>
-      <c r="BI13" s="14"/>
-      <c r="BJ13" s="14"/>
-      <c r="BK13" s="14"/>
-      <c r="BL13" s="14"/>
-      <c r="BM13" s="14"/>
-      <c r="BN13" s="14"/>
-      <c r="BO13" s="14"/>
-      <c r="BP13" s="14"/>
-      <c r="BQ13" s="14"/>
-      <c r="BR13" s="14"/>
+      <c r="G13" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="L13" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="26"/>
+      <c r="S13" s="26"/>
+      <c r="T13" s="26"/>
+      <c r="U13" s="26"/>
+      <c r="V13" s="26"/>
+      <c r="W13" s="26"/>
+      <c r="X13" s="26"/>
+      <c r="Y13" s="26"/>
+      <c r="Z13" s="26"/>
+      <c r="AA13" s="26"/>
+      <c r="AB13" s="26"/>
+      <c r="AC13" s="26"/>
+      <c r="AD13" s="26"/>
+      <c r="AE13" s="26"/>
+      <c r="AF13" s="26"/>
+      <c r="AG13" s="26"/>
+      <c r="AH13" s="26"/>
+      <c r="AI13" s="26"/>
+      <c r="AJ13" s="26"/>
+      <c r="AK13" s="26"/>
+      <c r="AL13" s="26"/>
+      <c r="AM13" s="26"/>
+      <c r="AN13" s="26"/>
+      <c r="AO13" s="26"/>
+      <c r="AP13" s="26"/>
+      <c r="AQ13" s="26"/>
+      <c r="AR13" s="26"/>
+      <c r="AS13" s="26"/>
+      <c r="AT13" s="26"/>
+      <c r="AU13" s="26"/>
+      <c r="AV13" s="26"/>
+      <c r="AW13" s="26"/>
+      <c r="AX13" s="26"/>
+      <c r="AY13" s="26"/>
+      <c r="AZ13" s="26"/>
+      <c r="BA13" s="26"/>
+      <c r="BB13" s="26"/>
+      <c r="BC13" s="26"/>
+      <c r="BD13" s="26"/>
+      <c r="BE13" s="26"/>
+      <c r="BF13" s="26"/>
+      <c r="BG13" s="26"/>
+      <c r="BH13" s="26"/>
+      <c r="BI13" s="26"/>
+      <c r="BJ13" s="26"/>
+      <c r="BK13" s="26"/>
+      <c r="BL13" s="26"/>
+      <c r="BM13" s="26"/>
+      <c r="BN13" s="26"/>
+      <c r="BO13" s="26"/>
+      <c r="BP13" s="26"/>
+      <c r="BQ13" s="26"/>
+      <c r="BR13" s="26"/>
     </row>
     <row r="14" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="64" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="11" t="s">
@@ -2553,7 +2580,7 @@
       <c r="BR14" s="14"/>
     </row>
     <row r="15" spans="1:70" s="39" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="64" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="39" t="s">
@@ -2653,7 +2680,7 @@
       <c r="BR15" s="26"/>
     </row>
     <row r="16" spans="1:70" x14ac:dyDescent="0.45">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="51" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="14" t="s">
@@ -2694,6 +2721,7 @@
       </c>
     </row>
     <row r="17" spans="1:70" s="29" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="74"/>
       <c r="B17" s="29" t="s">
         <v>79</v>
       </c>
@@ -2785,7 +2813,7 @@
       <c r="BR17" s="26"/>
     </row>
     <row r="18" spans="1:70" s="39" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="64" t="s">
         <v>27</v>
       </c>
       <c r="B18" s="39" t="s">
@@ -2883,7 +2911,7 @@
       <c r="BR18" s="26"/>
     </row>
     <row r="19" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="64" t="s">
         <v>28</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -2979,7 +3007,7 @@
       <c r="BR19" s="14"/>
     </row>
     <row r="20" spans="1:70" x14ac:dyDescent="0.45">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="51" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="14" t="s">
@@ -3026,6 +3054,7 @@
       </c>
     </row>
     <row r="21" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="51"/>
       <c r="B21" s="26" t="s">
         <v>83</v>
       </c>
@@ -3065,6 +3094,7 @@
       <c r="P21" s="28"/>
     </row>
     <row r="22" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="51"/>
       <c r="B22" s="26" t="s">
         <v>84</v>
       </c>
@@ -3100,42 +3130,48 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.45">
-      <c r="B23" s="14" t="s">
+    <row r="23" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="51"/>
+      <c r="B23" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="E23" s="16">
+      <c r="E23" s="27">
         <v>45002.429236111107</v>
       </c>
-      <c r="F23" s="16">
+      <c r="F23" s="27">
         <v>45002.440057870372</v>
       </c>
-      <c r="G23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M23" s="2" t="s">
+      <c r="G23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M23" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="N23" s="2" t="s">
+      <c r="N23" s="8" t="s">
         <v>189</v>
       </c>
+      <c r="O23" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="P23" s="28"/>
     </row>
     <row r="24" spans="1:70" s="29" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="74"/>
       <c r="B24" s="29" t="s">
         <v>86</v>
       </c>
@@ -3273,6 +3309,7 @@
       <c r="P25" s="28"/>
     </row>
     <row r="26" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="51"/>
       <c r="B26" s="26" t="s">
         <v>89</v>
       </c>
@@ -3307,6 +3344,7 @@
       </c>
     </row>
     <row r="27" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="51"/>
       <c r="B27" s="26" t="s">
         <v>88</v>
       </c>
@@ -3340,34 +3378,39 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.45">
-      <c r="B28" s="14" t="s">
+    <row r="28" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="51"/>
+      <c r="B28" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="E28" s="16">
+      <c r="E28" s="27">
         <v>45002.342222222222</v>
       </c>
-      <c r="F28" s="16">
+      <c r="F28" s="27">
         <v>45002.472083333327</v>
       </c>
-      <c r="G28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="G28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="28"/>
     </row>
     <row r="29" spans="1:70" x14ac:dyDescent="0.45">
       <c r="B29" s="14" t="s">
@@ -3428,6 +3471,7 @@
       </c>
     </row>
     <row r="31" spans="1:70" s="24" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="74"/>
       <c r="B31" s="24" t="s">
         <v>253</v>
       </c>
@@ -3593,6 +3637,7 @@
       <c r="P33" s="55"/>
     </row>
     <row r="34" spans="1:70" s="29" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="74"/>
       <c r="B34" s="29" t="s">
         <v>95</v>
       </c>
@@ -3684,7 +3729,7 @@
       <c r="BR34" s="26"/>
     </row>
     <row r="35" spans="1:70" s="39" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="39" t="s">
+      <c r="A35" s="64" t="s">
         <v>13</v>
       </c>
       <c r="B35" s="39" t="s">
@@ -3782,7 +3827,7 @@
       <c r="BR35" s="26"/>
     </row>
     <row r="36" spans="1:70" x14ac:dyDescent="0.45">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="51" t="s">
         <v>14</v>
       </c>
       <c r="B36" s="14" t="s">
@@ -3820,6 +3865,7 @@
       </c>
     </row>
     <row r="37" spans="1:70" s="29" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="74"/>
       <c r="B37" s="29" t="s">
         <v>98</v>
       </c>
@@ -3909,7 +3955,7 @@
       <c r="BR37" s="26"/>
     </row>
     <row r="38" spans="1:70" x14ac:dyDescent="0.45">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="51" t="s">
         <v>15</v>
       </c>
       <c r="B38" s="14" t="s">
@@ -4034,6 +4080,7 @@
       </c>
     </row>
     <row r="42" spans="1:70" s="24" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="74"/>
       <c r="B42" s="24" t="s">
         <v>103</v>
       </c>
@@ -4121,7 +4168,7 @@
       <c r="BR42" s="14"/>
     </row>
     <row r="43" spans="1:70" s="39" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="64" t="s">
         <v>29</v>
       </c>
       <c r="B43" s="39" t="s">
@@ -4223,7 +4270,7 @@
       <c r="BR43" s="26"/>
     </row>
     <row r="44" spans="1:70" x14ac:dyDescent="0.45">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="51" t="s">
         <v>30</v>
       </c>
       <c r="B44" s="14" t="s">
@@ -4261,6 +4308,7 @@
       </c>
     </row>
     <row r="45" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="51"/>
       <c r="B45" s="26" t="s">
         <v>107</v>
       </c>
@@ -4295,95 +4343,96 @@
       </c>
       <c r="P45" s="28"/>
     </row>
-    <row r="46" spans="1:70" s="24" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B46" s="24" t="s">
+    <row r="46" spans="1:70" s="29" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="74"/>
+      <c r="B46" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="E46" s="25">
+      <c r="E46" s="30">
         <v>45119.398460648154</v>
       </c>
-      <c r="F46" s="25">
+      <c r="F46" s="30">
         <v>45119.429537037038</v>
       </c>
-      <c r="G46" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J46" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K46" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L46" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M46" s="5"/>
-      <c r="N46" s="5"/>
-      <c r="O46" s="5"/>
-      <c r="P46" s="13"/>
-      <c r="Q46" s="14"/>
-      <c r="R46" s="14"/>
-      <c r="S46" s="14"/>
-      <c r="T46" s="14"/>
-      <c r="U46" s="14"/>
-      <c r="V46" s="14"/>
-      <c r="W46" s="14"/>
-      <c r="X46" s="14"/>
-      <c r="Y46" s="14"/>
-      <c r="Z46" s="14"/>
-      <c r="AA46" s="14"/>
-      <c r="AB46" s="14"/>
-      <c r="AC46" s="14"/>
-      <c r="AD46" s="14"/>
-      <c r="AE46" s="14"/>
-      <c r="AF46" s="14"/>
-      <c r="AG46" s="14"/>
-      <c r="AH46" s="14"/>
-      <c r="AI46" s="14"/>
-      <c r="AJ46" s="14"/>
-      <c r="AK46" s="14"/>
-      <c r="AL46" s="14"/>
-      <c r="AM46" s="14"/>
-      <c r="AN46" s="14"/>
-      <c r="AO46" s="14"/>
-      <c r="AP46" s="14"/>
-      <c r="AQ46" s="14"/>
-      <c r="AR46" s="14"/>
-      <c r="AS46" s="14"/>
-      <c r="AT46" s="14"/>
-      <c r="AU46" s="14"/>
-      <c r="AV46" s="14"/>
-      <c r="AW46" s="14"/>
-      <c r="AX46" s="14"/>
-      <c r="AY46" s="14"/>
-      <c r="AZ46" s="14"/>
-      <c r="BA46" s="14"/>
-      <c r="BB46" s="14"/>
-      <c r="BC46" s="14"/>
-      <c r="BD46" s="14"/>
-      <c r="BE46" s="14"/>
-      <c r="BF46" s="14"/>
-      <c r="BG46" s="14"/>
-      <c r="BH46" s="14"/>
-      <c r="BI46" s="14"/>
-      <c r="BJ46" s="14"/>
-      <c r="BK46" s="14"/>
-      <c r="BL46" s="14"/>
-      <c r="BM46" s="14"/>
-      <c r="BN46" s="14"/>
-      <c r="BO46" s="14"/>
-      <c r="BP46" s="14"/>
-      <c r="BQ46" s="14"/>
-      <c r="BR46" s="14"/>
+      <c r="G46" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H46" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I46" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J46" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K46" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L46" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="M46" s="10"/>
+      <c r="N46" s="10"/>
+      <c r="O46" s="10"/>
+      <c r="P46" s="28"/>
+      <c r="Q46" s="26"/>
+      <c r="R46" s="26"/>
+      <c r="S46" s="26"/>
+      <c r="T46" s="26"/>
+      <c r="U46" s="26"/>
+      <c r="V46" s="26"/>
+      <c r="W46" s="26"/>
+      <c r="X46" s="26"/>
+      <c r="Y46" s="26"/>
+      <c r="Z46" s="26"/>
+      <c r="AA46" s="26"/>
+      <c r="AB46" s="26"/>
+      <c r="AC46" s="26"/>
+      <c r="AD46" s="26"/>
+      <c r="AE46" s="26"/>
+      <c r="AF46" s="26"/>
+      <c r="AG46" s="26"/>
+      <c r="AH46" s="26"/>
+      <c r="AI46" s="26"/>
+      <c r="AJ46" s="26"/>
+      <c r="AK46" s="26"/>
+      <c r="AL46" s="26"/>
+      <c r="AM46" s="26"/>
+      <c r="AN46" s="26"/>
+      <c r="AO46" s="26"/>
+      <c r="AP46" s="26"/>
+      <c r="AQ46" s="26"/>
+      <c r="AR46" s="26"/>
+      <c r="AS46" s="26"/>
+      <c r="AT46" s="26"/>
+      <c r="AU46" s="26"/>
+      <c r="AV46" s="26"/>
+      <c r="AW46" s="26"/>
+      <c r="AX46" s="26"/>
+      <c r="AY46" s="26"/>
+      <c r="AZ46" s="26"/>
+      <c r="BA46" s="26"/>
+      <c r="BB46" s="26"/>
+      <c r="BC46" s="26"/>
+      <c r="BD46" s="26"/>
+      <c r="BE46" s="26"/>
+      <c r="BF46" s="26"/>
+      <c r="BG46" s="26"/>
+      <c r="BH46" s="26"/>
+      <c r="BI46" s="26"/>
+      <c r="BJ46" s="26"/>
+      <c r="BK46" s="26"/>
+      <c r="BL46" s="26"/>
+      <c r="BM46" s="26"/>
+      <c r="BN46" s="26"/>
+      <c r="BO46" s="26"/>
+      <c r="BP46" s="26"/>
+      <c r="BQ46" s="26"/>
+      <c r="BR46" s="26"/>
     </row>
     <row r="47" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B47" s="11" t="s">
@@ -4481,7 +4530,7 @@
       <c r="BR47" s="14"/>
     </row>
     <row r="48" spans="1:70" x14ac:dyDescent="0.45">
-      <c r="A48" s="14" t="s">
+      <c r="A48" s="51" t="s">
         <v>32</v>
       </c>
       <c r="B48" s="14" t="s">
@@ -4525,6 +4574,7 @@
       </c>
     </row>
     <row r="49" spans="1:70" s="29" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="74"/>
       <c r="B49" s="29" t="s">
         <v>255</v>
       </c>
@@ -4614,7 +4664,7 @@
       <c r="BR49" s="26"/>
     </row>
     <row r="50" spans="1:70" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="64" t="s">
         <v>33</v>
       </c>
       <c r="B50" s="11" t="s">
@@ -4710,7 +4760,7 @@
       <c r="BR50" s="14"/>
     </row>
     <row r="51" spans="1:70" s="44" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A51" s="44" t="s">
+      <c r="A51" s="75" t="s">
         <v>34</v>
       </c>
       <c r="B51" s="44" t="s">
@@ -4808,7 +4858,7 @@
       <c r="BR51" s="26"/>
     </row>
     <row r="52" spans="1:70" s="26" customFormat="1" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="26" t="s">
+      <c r="A52" s="51" t="s">
         <v>37</v>
       </c>
       <c r="B52" s="26" t="s">
@@ -4852,6 +4902,7 @@
       <c r="P52" s="28"/>
     </row>
     <row r="53" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A53" s="51"/>
       <c r="B53" s="26" t="s">
         <v>114</v>
       </c>
@@ -4885,6 +4936,7 @@
       <c r="P53" s="28"/>
     </row>
     <row r="54" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A54" s="51"/>
       <c r="B54" s="26" t="s">
         <v>115</v>
       </c>
@@ -4918,6 +4970,7 @@
       <c r="P54" s="28"/>
     </row>
     <row r="55" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A55" s="51"/>
       <c r="B55" s="26" t="s">
         <v>116</v>
       </c>
@@ -4951,6 +5004,7 @@
       <c r="P55" s="28"/>
     </row>
     <row r="56" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A56" s="51"/>
       <c r="B56" s="26" t="s">
         <v>117</v>
       </c>
@@ -4984,6 +5038,7 @@
       <c r="P56" s="28"/>
     </row>
     <row r="57" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A57" s="51"/>
       <c r="B57" s="26" t="s">
         <v>66</v>
       </c>
@@ -5017,6 +5072,7 @@
       <c r="P57" s="28"/>
     </row>
     <row r="58" spans="1:70" s="29" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A58" s="74"/>
       <c r="B58" s="29" t="s">
         <v>118</v>
       </c>
@@ -5104,7 +5160,7 @@
       <c r="BR58" s="26"/>
     </row>
     <row r="59" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="26" t="s">
+      <c r="A59" s="51" t="s">
         <v>36</v>
       </c>
       <c r="B59" s="26" t="s">
@@ -5148,6 +5204,7 @@
       <c r="P59" s="28"/>
     </row>
     <row r="60" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A60" s="51"/>
       <c r="B60" s="26" t="s">
         <v>120</v>
       </c>
@@ -5181,6 +5238,7 @@
       <c r="P60" s="28"/>
     </row>
     <row r="61" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A61" s="51"/>
       <c r="B61" s="26" t="s">
         <v>121</v>
       </c>
@@ -5214,6 +5272,7 @@
       <c r="P61" s="28"/>
     </row>
     <row r="62" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A62" s="51"/>
       <c r="B62" s="26" t="s">
         <v>122</v>
       </c>
@@ -5247,6 +5306,7 @@
       <c r="P62" s="28"/>
     </row>
     <row r="63" spans="1:70" s="29" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A63" s="74"/>
       <c r="B63" s="29" t="s">
         <v>123</v>
       </c>
@@ -5333,49 +5393,54 @@
       <c r="BQ63" s="26"/>
       <c r="BR63" s="26"/>
     </row>
-    <row r="64" spans="1:70" x14ac:dyDescent="0.45">
-      <c r="A64" s="14" t="s">
+    <row r="64" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A64" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="B64" s="14" t="s">
+      <c r="B64" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="C64" s="14" t="s">
+      <c r="C64" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="D64" s="14" t="s">
+      <c r="D64" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="E64" s="16">
+      <c r="E64" s="27">
         <v>42612.348975694447</v>
       </c>
-      <c r="F64" s="16">
+      <c r="F64" s="27">
         <v>42612.370908564822</v>
       </c>
-      <c r="G64" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H64" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I64" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J64" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K64" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L64" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M64" s="2" t="s">
+      <c r="G64" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H64" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I64" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J64" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K64" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L64" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M64" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="N64" s="15"/>
+      <c r="N64" s="48"/>
+      <c r="O64" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="P64" s="28"/>
     </row>
     <row r="65" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A65" s="51"/>
       <c r="B65" s="26" t="s">
         <v>125</v>
       </c>
@@ -5445,6 +5510,7 @@
       </c>
     </row>
     <row r="67" spans="1:70" s="24" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A67" s="74"/>
       <c r="B67" s="24" t="s">
         <v>127</v>
       </c>
@@ -5536,7 +5602,7 @@
       <c r="BR67" s="14"/>
     </row>
     <row r="68" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A68" s="26" t="s">
+      <c r="A68" s="51" t="s">
         <v>39</v>
       </c>
       <c r="B68" s="26" t="s">
@@ -5580,6 +5646,7 @@
       <c r="P68" s="28"/>
     </row>
     <row r="69" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A69" s="51"/>
       <c r="B69" s="26" t="s">
         <v>129</v>
       </c>
@@ -5613,6 +5680,7 @@
       <c r="P69" s="28"/>
     </row>
     <row r="70" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A70" s="51"/>
       <c r="B70" s="26" t="s">
         <v>130</v>
       </c>
@@ -5646,6 +5714,7 @@
       <c r="P70" s="28"/>
     </row>
     <row r="71" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A71" s="51"/>
       <c r="B71" s="26" t="s">
         <v>131</v>
       </c>
@@ -5679,6 +5748,7 @@
       <c r="P71" s="28"/>
     </row>
     <row r="72" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A72" s="51"/>
       <c r="B72" s="26" t="s">
         <v>132</v>
       </c>
@@ -5712,6 +5782,7 @@
       <c r="P72" s="28"/>
     </row>
     <row r="73" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A73" s="51"/>
       <c r="B73" s="26" t="s">
         <v>133</v>
       </c>
@@ -5745,6 +5816,7 @@
       <c r="P73" s="28"/>
     </row>
     <row r="74" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A74" s="51"/>
       <c r="B74" s="26" t="s">
         <v>134</v>
       </c>
@@ -5778,6 +5850,7 @@
       <c r="P74" s="28"/>
     </row>
     <row r="75" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A75" s="51"/>
       <c r="B75" s="26" t="s">
         <v>135</v>
       </c>
@@ -5811,6 +5884,7 @@
       <c r="P75" s="28"/>
     </row>
     <row r="76" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A76" s="51"/>
       <c r="B76" s="26" t="s">
         <v>136</v>
       </c>
@@ -5844,6 +5918,7 @@
       <c r="P76" s="28"/>
     </row>
     <row r="77" spans="1:70" s="29" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A77" s="74"/>
       <c r="B77" s="29" t="s">
         <v>137</v>
       </c>
@@ -5930,48 +6005,54 @@
       <c r="BQ77" s="26"/>
       <c r="BR77" s="26"/>
     </row>
-    <row r="78" spans="1:70" x14ac:dyDescent="0.45">
-      <c r="A78" s="14" t="s">
+    <row r="78" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A78" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="B78" s="14" t="s">
+      <c r="B78" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="C78" s="14" t="s">
+      <c r="C78" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="D78" s="14" t="s">
+      <c r="D78" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="E78" s="16">
+      <c r="E78" s="27">
         <v>42612.397146990741</v>
       </c>
-      <c r="F78" s="16">
+      <c r="F78" s="27">
         <v>42612.39830439815</v>
       </c>
-      <c r="G78" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H78" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I78" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J78" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K78" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L78" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M78" s="2" t="s">
+      <c r="G78" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H78" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I78" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J78" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K78" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L78" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M78" s="8" t="s">
         <v>207</v>
       </c>
+      <c r="N78" s="8"/>
+      <c r="O78" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="P78" s="28"/>
     </row>
     <row r="79" spans="1:70" s="33" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A79" s="76"/>
       <c r="B79" s="33" t="s">
         <v>139</v>
       </c>
@@ -6061,7 +6142,7 @@
       <c r="BR79" s="14"/>
     </row>
     <row r="80" spans="1:70" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A80" s="14" t="s">
+      <c r="A80" s="51" t="s">
         <v>40</v>
       </c>
       <c r="B80" s="14" t="s">
@@ -6151,6 +6232,7 @@
       </c>
     </row>
     <row r="83" spans="1:16" s="24" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A83" s="74"/>
       <c r="B83" s="24" t="s">
         <v>143</v>
       </c>
@@ -6183,7 +6265,7 @@
       <c r="P83" s="35"/>
     </row>
     <row r="84" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A84" s="14" t="s">
+      <c r="A84" s="51" t="s">
         <v>41</v>
       </c>
       <c r="B84" s="14" t="s">
@@ -6253,6 +6335,7 @@
       </c>
     </row>
     <row r="86" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A86" s="51"/>
       <c r="B86" s="26" t="s">
         <v>146</v>
       </c>
@@ -6345,6 +6428,7 @@
       </c>
     </row>
     <row r="89" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A89" s="51"/>
       <c r="B89" s="26" t="s">
         <v>149</v>
       </c>
@@ -6411,6 +6495,7 @@
       </c>
     </row>
     <row r="91" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A91" s="51"/>
       <c r="B91" s="26" t="s">
         <v>67</v>
       </c>
@@ -6560,6 +6645,7 @@
       </c>
     </row>
     <row r="96" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A96" s="51"/>
       <c r="B96" s="26" t="s">
         <v>155</v>
       </c>
@@ -6592,7 +6678,7 @@
       </c>
       <c r="P96" s="28"/>
     </row>
-    <row r="97" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B97" s="14" t="s">
         <v>156</v>
       </c>
@@ -6624,36 +6710,43 @@
         <v>196</v>
       </c>
     </row>
-    <row r="98" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="B98" s="14" t="s">
+    <row r="98" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A98" s="51"/>
+      <c r="B98" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="E98" s="16">
+      <c r="E98" s="27">
         <v>43346.276759259257</v>
       </c>
-      <c r="G98" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H98" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I98" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J98" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K98" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L98" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M98" s="2" t="s">
+      <c r="G98" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H98" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I98" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J98" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K98" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L98" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M98" s="8" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="99" spans="2:16" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="N98" s="8"/>
+      <c r="O98" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="P98" s="28"/>
+    </row>
+    <row r="99" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A99" s="51"/>
       <c r="B99" s="26" t="s">
         <v>158</v>
       </c>
@@ -6687,7 +6780,8 @@
       </c>
       <c r="P99" s="28"/>
     </row>
-    <row r="100" spans="2:16" s="26" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A100" s="51"/>
       <c r="B100" s="26" t="s">
         <v>159</v>
       </c>
@@ -6721,7 +6815,8 @@
       </c>
       <c r="P100" s="28"/>
     </row>
-    <row r="101" spans="2:16" s="26" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A101" s="51"/>
       <c r="B101" s="26" t="s">
         <v>160</v>
       </c>
@@ -6757,7 +6852,8 @@
       </c>
       <c r="P101" s="28"/>
     </row>
-    <row r="102" spans="2:16" s="26" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A102" s="51"/>
       <c r="B102" s="26" t="s">
         <v>161</v>
       </c>
@@ -6793,7 +6889,8 @@
       </c>
       <c r="P102" s="28"/>
     </row>
-    <row r="103" spans="2:16" s="26" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A103" s="51"/>
       <c r="B103" s="26" t="s">
         <v>162</v>
       </c>
@@ -6829,7 +6926,8 @@
       </c>
       <c r="P103" s="28"/>
     </row>
-    <row r="104" spans="2:16" s="26" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A104" s="51"/>
       <c r="B104" s="26" t="s">
         <v>163</v>
       </c>
@@ -6865,7 +6963,7 @@
       </c>
       <c r="P104" s="28"/>
     </row>
-    <row r="105" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B105" s="14" t="s">
         <v>164</v>
       </c>
@@ -6894,7 +6992,8 @@
         <v>231</v>
       </c>
     </row>
-    <row r="106" spans="2:16" s="26" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A106" s="51"/>
       <c r="B106" s="26" t="s">
         <v>165</v>
       </c>
@@ -6930,7 +7029,7 @@
       </c>
       <c r="P106" s="28"/>
     </row>
-    <row r="107" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B107" s="14" t="s">
         <v>166</v>
       </c>
@@ -6956,7 +7055,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B108" s="14" t="s">
         <v>167</v>
       </c>
@@ -6982,7 +7081,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B109" s="14" t="s">
         <v>168</v>
       </c>
@@ -7008,39 +7107,44 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="B110" s="14" t="s">
+    <row r="110" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A110" s="51"/>
+      <c r="B110" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="E110" s="16">
+      <c r="E110" s="27">
         <v>43363.818651620371</v>
       </c>
-      <c r="G110" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H110" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I110" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J110" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K110" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L110" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M110" s="2" t="s">
+      <c r="G110" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H110" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I110" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J110" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K110" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L110" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M110" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="N110" s="2" t="s">
+      <c r="N110" s="8" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="111" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="O110" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="P110" s="28"/>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B111" s="14" t="s">
         <v>170</v>
       </c>
@@ -7069,7 +7173,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="112" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B112" s="14" t="s">
         <v>171</v>
       </c>
@@ -7095,37 +7199,42 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="B113" s="14" t="s">
+    <row r="113" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A113" s="51"/>
+      <c r="B113" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="E113" s="16">
+      <c r="E113" s="27">
         <v>43367.151695601853</v>
       </c>
-      <c r="G113" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H113" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I113" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J113" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K113" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L113" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M113" s="2" t="s">
+      <c r="G113" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H113" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I113" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J113" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K113" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L113" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M113" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="N113" s="2" t="s">
+      <c r="N113" s="8" t="s">
         <v>194</v>
       </c>
+      <c r="O113" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="P113" s="28"/>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B114" s="14" t="s">
@@ -7247,6 +7356,7 @@
       </c>
     </row>
     <row r="118" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A118" s="51"/>
       <c r="B118" s="26" t="s">
         <v>177</v>
       </c>
@@ -7277,10 +7387,13 @@
       <c r="N118" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="O118" s="8"/>
+      <c r="O118" s="8" t="s">
+        <v>266</v>
+      </c>
       <c r="P118" s="28"/>
     </row>
     <row r="119" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A119" s="51"/>
       <c r="B119" s="26" t="s">
         <v>178</v>
       </c>
@@ -7309,10 +7422,13 @@
         <v>241</v>
       </c>
       <c r="N119" s="8"/>
-      <c r="O119" s="8"/>
+      <c r="O119" s="8" t="s">
+        <v>266</v>
+      </c>
       <c r="P119" s="28"/>
     </row>
     <row r="120" spans="1:16" s="26" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A120" s="51"/>
       <c r="B120" s="26" t="s">
         <v>179</v>
       </c>
@@ -7343,7 +7459,9 @@
       <c r="N120" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="O120" s="8"/>
+      <c r="O120" s="8" t="s">
+        <v>266</v>
+      </c>
       <c r="P120" s="28"/>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.45">
@@ -7379,6 +7497,7 @@
       </c>
     </row>
     <row r="122" spans="1:16" s="24" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A122" s="74"/>
       <c r="B122" s="14" t="s">
         <v>181</v>
       </c>
@@ -7413,7 +7532,7 @@
       <c r="P122" s="35"/>
     </row>
     <row r="123" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A123" s="11" t="s">
+      <c r="A123" s="64" t="s">
         <v>42</v>
       </c>
       <c r="B123" s="11" t="s">
@@ -7454,7 +7573,7 @@
       <c r="P123" s="36"/>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A124" s="14" t="s">
+      <c r="A124" s="51" t="s">
         <v>43</v>
       </c>
       <c r="B124" s="14" t="s">
@@ -7573,6 +7692,7 @@
       </c>
     </row>
     <row r="128" spans="1:16" s="33" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A128" s="76"/>
       <c r="B128" s="33" t="s">
         <v>187</v>
       </c>
@@ -7614,10 +7734,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DDFDEA-2838-4C23-95EB-05B925C7BB88}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7711,28 +7831,26 @@
       </c>
     </row>
     <row r="7" spans="1:5" s="68" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="66" t="s">
+      <c r="A7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="62" t="s">
         <v>257</v>
       </c>
-      <c r="D7" s="67" t="s">
+      <c r="D7" s="61" t="s">
         <v>260</v>
       </c>
-      <c r="E7" s="68" t="s">
-        <v>267</v>
-      </c>
+      <c r="E7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>76</v>
+      <c r="A8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="C8" s="62" t="s">
         <v>257</v>
@@ -7742,13 +7860,13 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="62" t="s">
+      <c r="A9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="63" t="s">
         <v>257</v>
       </c>
       <c r="D9" s="61" t="s">
@@ -7757,143 +7875,130 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="63" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="62" t="s">
         <v>257</v>
       </c>
       <c r="D10" s="61" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" s="68" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C11" t="s">
+        <v>258</v>
+      </c>
+      <c r="D11" s="57" t="s">
+        <v>260</v>
+      </c>
+      <c r="E11"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" t="s">
         <v>257</v>
       </c>
-      <c r="D11" s="57" t="s">
+      <c r="D12" s="57" t="s">
         <v>261</v>
       </c>
-      <c r="E11" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="68" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="29"/>
-      <c r="B12" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="70" t="s">
+      <c r="E12" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" s="24"/>
+      <c r="B13" s="24" t="s">
+        <v>253</v>
+      </c>
+      <c r="C13" s="63" t="s">
+        <v>258</v>
+      </c>
+      <c r="D13" s="58" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" s="64" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="64" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="62" t="s">
         <v>257</v>
       </c>
-      <c r="D12" s="71" t="s">
-        <v>261</v>
-      </c>
-      <c r="E12" s="68" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="68" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="68" t="s">
+      <c r="D14" s="61" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="62" t="s">
         <v>258</v>
       </c>
-      <c r="D13" s="69" t="s">
+      <c r="D15" s="61" t="s">
         <v>260</v>
       </c>
-      <c r="E13" s="68" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" t="s">
         <v>258</v>
       </c>
-      <c r="D14" s="57" t="s">
+      <c r="D16" s="57" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="C15" t="s">
-        <v>257</v>
-      </c>
-      <c r="D15" s="57" t="s">
-        <v>261</v>
-      </c>
-      <c r="E15" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24" t="s">
-        <v>253</v>
-      </c>
-      <c r="C16" s="63" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" t="s">
         <v>258</v>
       </c>
-      <c r="D16" s="58" t="s">
+      <c r="D17" s="57" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A17" s="64" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="64" t="s">
-        <v>94</v>
-      </c>
-      <c r="C17" s="62" t="s">
-        <v>257</v>
-      </c>
-      <c r="D17" s="61" t="s">
-        <v>261</v>
-      </c>
-      <c r="E17" t="s">
-        <v>268</v>
-      </c>
-    </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A18" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C18" s="62" t="s">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" t="s">
         <v>258</v>
       </c>
-      <c r="D18" s="61" t="s">
+      <c r="D18" s="57" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A19" s="14" t="s">
-        <v>15</v>
-      </c>
+      <c r="A19" s="14"/>
       <c r="B19" s="14" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C19" t="s">
         <v>258</v>
@@ -7903,21 +8008,23 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="A20" s="24"/>
+      <c r="B20" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="63" t="s">
         <v>258</v>
       </c>
-      <c r="D20" s="57" t="s">
+      <c r="D20" s="58" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A21" s="14"/>
+      <c r="A21" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="B21" s="14" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C21" t="s">
         <v>258</v>
@@ -7926,128 +8033,125 @@
         <v>260</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="C22" t="s">
+    <row r="22" spans="1:5" s="68" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C22" s="62" t="s">
+        <v>257</v>
+      </c>
+      <c r="D22" s="61" t="s">
+        <v>260</v>
+      </c>
+      <c r="E22"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="66" t="s">
+        <v>257</v>
+      </c>
+      <c r="D23" s="67" t="s">
+        <v>261</v>
+      </c>
+      <c r="E23" s="68" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="68" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A24" s="59" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" s="60" t="s">
         <v>258</v>
       </c>
-      <c r="D22" s="57" t="s">
+      <c r="D24" s="65" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A23" s="24"/>
-      <c r="B23" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="C23" s="63" t="s">
+      <c r="E24"/>
+    </row>
+    <row r="25" spans="1:5" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="C25" t="s">
+        <v>257</v>
+      </c>
+      <c r="D25" s="57" t="s">
+        <v>260</v>
+      </c>
+      <c r="E25" s="69"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" t="s">
         <v>258</v>
       </c>
-      <c r="D23" s="58" t="s">
+      <c r="D26" s="57" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A24" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C24" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" s="14"/>
+      <c r="B27" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C27" t="s">
         <v>258</v>
       </c>
-      <c r="D24" s="57" t="s">
+      <c r="D27" s="57" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="68" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="29"/>
-      <c r="B25" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="C25" s="70" t="s">
+    <row r="28" spans="1:5" s="68" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="29"/>
+      <c r="B28" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="C28" s="70" t="s">
         <v>258</v>
       </c>
-      <c r="D25" s="71" t="s">
+      <c r="D28" s="71" t="s">
         <v>260</v>
       </c>
-      <c r="E25" s="68" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="C26" s="62" t="s">
-        <v>257</v>
-      </c>
-      <c r="D26" s="61" t="s">
-        <v>261</v>
-      </c>
-      <c r="E26" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="68" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="C27" s="66" t="s">
-        <v>257</v>
-      </c>
-      <c r="D27" s="67" t="s">
-        <v>261</v>
-      </c>
-      <c r="E27" s="68" t="s">
+      <c r="E28" s="68" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A28" s="59" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="59" t="s">
-        <v>110</v>
-      </c>
-      <c r="C28" s="60" t="s">
-        <v>258</v>
-      </c>
-      <c r="D28" s="65" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C29" t="s">
         <v>257</v>
       </c>
       <c r="D29" s="57" t="s">
-        <v>261</v>
-      </c>
-      <c r="E29" s="72" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" s="14"/>
       <c r="B30" s="14" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C30" t="s">
         <v>258</v>
@@ -8057,9 +8161,9 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A31" s="14"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="14" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C31" t="s">
         <v>258</v>
@@ -8069,35 +8173,33 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A32" s="24"/>
-      <c r="B32" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="C32" s="63" t="s">
+      <c r="A32" s="14"/>
+      <c r="B32" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C32" t="s">
         <v>258</v>
       </c>
-      <c r="D32" s="58" t="s">
+      <c r="D32" s="57" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A33" s="14" t="s">
-        <v>41</v>
-      </c>
+      <c r="A33" s="14"/>
       <c r="B33" s="14" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="C33" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D33" s="57" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A34" s="14"/>
+      <c r="A34" s="26"/>
       <c r="B34" s="14" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C34" t="s">
         <v>258</v>
@@ -8107,9 +8209,9 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A35" s="26"/>
+      <c r="A35" s="14"/>
       <c r="B35" s="14" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="C35" t="s">
         <v>258</v>
@@ -8119,9 +8221,9 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A36" s="14"/>
+      <c r="A36" s="26"/>
       <c r="B36" s="14" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C36" t="s">
         <v>258</v>
@@ -8133,19 +8235,19 @@
     <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" s="14"/>
       <c r="B37" s="14" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C37" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D37" s="57" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A38" s="26"/>
+      <c r="A38" s="14"/>
       <c r="B38" s="14" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C38" t="s">
         <v>258</v>
@@ -8154,22 +8256,25 @@
         <v>260</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="C39" t="s">
-        <v>258</v>
-      </c>
-      <c r="D39" s="57" t="s">
-        <v>260</v>
+    <row r="39" spans="1:5" s="68" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="26"/>
+      <c r="B39" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="C39" s="68" t="s">
+        <v>257</v>
+      </c>
+      <c r="D39" s="72" t="s">
+        <v>261</v>
+      </c>
+      <c r="E39" s="68" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" s="26"/>
       <c r="B40" s="14" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="C40" t="s">
         <v>258</v>
@@ -8181,61 +8286,55 @@
     <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" s="14"/>
       <c r="B41" s="14" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="C41" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D41" s="57" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" s="14"/>
       <c r="B42" s="14" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="C42" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D42" s="57" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="68" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" s="26"/>
-      <c r="B43" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="C43" s="68" t="s">
-        <v>257</v>
-      </c>
-      <c r="D43" s="69" t="s">
-        <v>261</v>
-      </c>
-      <c r="E43" s="68" t="s">
-        <v>262</v>
+      <c r="B43" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="C43" t="s">
+        <v>258</v>
+      </c>
+      <c r="D43" s="57" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A44" s="14"/>
+      <c r="A44" s="26"/>
       <c r="B44" s="14" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="C44" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D44" s="57" t="s">
-        <v>261</v>
-      </c>
-      <c r="E44" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" s="26"/>
       <c r="B45" s="14" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="C45" t="s">
         <v>258</v>
@@ -8245,9 +8344,9 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A46" s="14"/>
+      <c r="A46" s="26"/>
       <c r="B46" s="14" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="C46" t="s">
         <v>258</v>
@@ -8256,42 +8355,201 @@
         <v>260</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A47" s="14"/>
-      <c r="B47" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="C47" t="s">
+    <row r="47" spans="1:5" s="68" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="26"/>
+      <c r="B47" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="C47" s="68" t="s">
         <v>257</v>
       </c>
-      <c r="D47" s="57" t="s">
+      <c r="D47" s="72" t="s">
         <v>261</v>
+      </c>
+      <c r="E47" s="68" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" s="26"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B48" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="C48" t="s">
+        <v>258</v>
+      </c>
+      <c r="D48" s="57" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="68" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A49" s="26"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A50" s="26"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A51" s="14"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A52" s="26"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B49" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="C49" s="68" t="s">
+        <v>257</v>
+      </c>
+      <c r="D49" s="72" t="s">
+        <v>261</v>
+      </c>
+      <c r="E49" s="68" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="68" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="29"/>
+      <c r="B50" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="C50" s="70" t="s">
+        <v>257</v>
+      </c>
+      <c r="D50" s="71" t="s">
+        <v>261</v>
+      </c>
+      <c r="E50" s="68" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="69" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="64" t="s">
+        <v>42</v>
+      </c>
+      <c r="B51" s="39" t="s">
+        <v>182</v>
+      </c>
+      <c r="C51" s="66" t="s">
+        <v>257</v>
+      </c>
+      <c r="D51" s="67" t="s">
+        <v>261</v>
+      </c>
+      <c r="E51" s="68" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A52" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="C52" t="s">
+        <v>257</v>
+      </c>
+      <c r="D52" s="57" t="s">
+        <v>260</v>
+      </c>
+      <c r="E52" s="69" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" s="14"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B53" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C53" t="s">
+        <v>258</v>
+      </c>
+      <c r="D53" s="57" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" s="14"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B54" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="C54" t="s">
+        <v>257</v>
+      </c>
+      <c r="D54" s="57" t="s">
+        <v>260</v>
+      </c>
+      <c r="E54" s="69" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" s="14"/>
-    </row>
+      <c r="B55" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="C55" s="68" t="s">
+        <v>257</v>
+      </c>
+      <c r="D55" s="72" t="s">
+        <v>261</v>
+      </c>
+      <c r="E55" s="68" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A56" s="60"/>
+      <c r="B56" s="78" t="s">
+        <v>187</v>
+      </c>
+      <c r="C56" s="79" t="s">
+        <v>257</v>
+      </c>
+      <c r="D56" s="80" t="s">
+        <v>261</v>
+      </c>
+      <c r="E56" s="68" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>38</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C57" t="s">
+        <v>257</v>
+      </c>
+      <c r="D57" s="57" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A58" s="63"/>
+      <c r="B58" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C58" s="63" t="s">
+        <v>257</v>
+      </c>
+      <c r="D58" s="58" t="s">
+        <v>260</v>
+      </c>
+      <c r="E58" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A59" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="B59" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="C59" s="60" t="s">
+        <v>257</v>
+      </c>
+      <c r="D59" s="77" t="s">
+        <v>260</v>
+      </c>
+      <c r="E59" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updates to Thesis Draft
Edits from the last month
</commit_message>
<xml_diff>
--- a/Analysis_Progress.xlsx
+++ b/Analysis_Progress.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9d4c4f1623d30376/Documents/GitHub/Rissos_Geographic_Variation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9D4C4F1623D30376/Documents/GitHub/Rissos_Geographic_Variation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1883" documentId="8_{C4C2D1DD-6DD6-49C2-8C12-51DEE2FC981A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{606A2E8C-4569-4976-BFD7-58053B744B7E}"/>
+  <xr:revisionPtr revIDLastSave="1884" documentId="8_{C4C2D1DD-6DD6-49C2-8C12-51DEE2FC981A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9A12DD1-3CE9-4E8D-B87F-7E20ED87BAB0}"/>
   <bookViews>
-    <workbookView xWindow="4253" yWindow="788" windowWidth="10492" windowHeight="11850" xr2:uid="{8391C37B-1672-4229-8478-45F991E75901}"/>
+    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="12863" firstSheet="1" activeTab="1" xr2:uid="{8391C37B-1672-4229-8478-45F991E75901}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Progress" sheetId="1" r:id="rId1"/>
@@ -1305,10 +1305,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1628,7 +1624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A18B98B-9FEB-4551-88CC-94F33BC1EF6E}">
   <dimension ref="A1:BR129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M11" zoomScale="57" zoomScaleNormal="45" workbookViewId="0">
+    <sheetView zoomScale="57" zoomScaleNormal="45" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -7738,8 +7734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DDFDEA-2838-4C23-95EB-05B925C7BB88}">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="82" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7798,7 +7794,7 @@
         <v>64</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D4" s="58" t="s">
         <v>260</v>

</xml_diff>